<commit_message>
ulteriori modifiche per pulire foglio excel da print precedenti
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,49 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimmy.carradore\Desktop\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15915" windowHeight="12270"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="15915" windowHeight="12270" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -62,22 +54,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -365,27 +416,1029 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:ALK1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EJ1" workbookViewId="0">
-      <selection activeCell="EJ1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:AF1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="154" max="154" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="155" max="155" width="27.7109375" customWidth="1"/>
-    <col min="156" max="156" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="21.140625" bestFit="1" customWidth="1"/>
+    <col width="27.85546875" bestFit="1" customWidth="1" min="154" max="154"/>
+    <col width="27.7109375" customWidth="1" min="155" max="155"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" min="156" max="156"/>
+    <col width="22.140625" bestFit="1" customWidth="1" min="157" max="157"/>
+    <col width="21.140625" bestFit="1" customWidth="1" min="158" max="158"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr"/>
+      <c r="C1" s="1" t="inlineStr"/>
+      <c r="D1" s="1" t="inlineStr"/>
+      <c r="E1" s="1" t="inlineStr"/>
+      <c r="F1" s="1" t="inlineStr"/>
+      <c r="G1" s="1" t="inlineStr"/>
+      <c r="H1" s="1" t="inlineStr"/>
+      <c r="I1" s="1" t="inlineStr"/>
+      <c r="J1" s="1" t="inlineStr"/>
+      <c r="K1" s="1" t="inlineStr"/>
+      <c r="L1" s="1" t="inlineStr"/>
+      <c r="M1" s="1" t="inlineStr"/>
+      <c r="N1" s="1" t="inlineStr"/>
+      <c r="O1" s="1" t="inlineStr"/>
+      <c r="P1" s="1" t="inlineStr"/>
+      <c r="Q1" s="1" t="inlineStr"/>
+      <c r="R1" s="1" t="inlineStr"/>
+      <c r="S1" s="1" t="inlineStr"/>
+      <c r="T1" s="1" t="inlineStr"/>
+      <c r="U1" s="1" t="inlineStr"/>
+      <c r="V1" s="1" t="inlineStr"/>
+      <c r="W1" s="1" t="inlineStr"/>
+      <c r="X1" s="1" t="inlineStr"/>
+      <c r="Y1" s="1" t="inlineStr"/>
+      <c r="Z1" s="1" t="inlineStr"/>
+      <c r="AA1" s="1" t="inlineStr"/>
+      <c r="AB1" s="1" t="inlineStr"/>
+      <c r="AC1" s="1" t="inlineStr"/>
+      <c r="AD1" s="1" t="inlineStr"/>
+      <c r="AE1" s="1" t="inlineStr"/>
+      <c r="AF1" s="1" t="inlineStr"/>
+      <c r="AG1" t="inlineStr"/>
+      <c r="AH1" t="inlineStr"/>
+      <c r="AI1" t="inlineStr"/>
+      <c r="AJ1" t="inlineStr"/>
+      <c r="AK1" t="inlineStr"/>
+      <c r="AL1" t="inlineStr"/>
+      <c r="AM1" t="inlineStr"/>
+      <c r="AN1" t="inlineStr"/>
+      <c r="AO1" t="inlineStr"/>
+      <c r="AP1" t="inlineStr"/>
+      <c r="AQ1" t="inlineStr"/>
+      <c r="AR1" t="inlineStr"/>
+      <c r="AS1" t="inlineStr"/>
+      <c r="AT1" t="inlineStr"/>
+      <c r="AU1" t="inlineStr"/>
+      <c r="AV1" t="inlineStr"/>
+      <c r="AW1" t="inlineStr"/>
+      <c r="AX1" t="inlineStr"/>
+      <c r="AY1" t="inlineStr"/>
+      <c r="AZ1" t="inlineStr"/>
+      <c r="BA1" t="inlineStr"/>
+      <c r="BB1" t="inlineStr"/>
+      <c r="BC1" t="inlineStr"/>
+      <c r="BD1" t="inlineStr"/>
+      <c r="BE1" t="inlineStr"/>
+      <c r="BF1" t="inlineStr"/>
+      <c r="BG1" t="inlineStr"/>
+      <c r="BH1" t="inlineStr"/>
+      <c r="BI1" t="inlineStr"/>
+      <c r="BJ1" t="inlineStr"/>
+      <c r="BK1" t="inlineStr"/>
+      <c r="BL1" t="inlineStr"/>
+      <c r="BM1" t="inlineStr"/>
+      <c r="BN1" t="inlineStr"/>
+      <c r="BO1" t="inlineStr"/>
+      <c r="BP1" t="inlineStr"/>
+      <c r="BQ1" t="inlineStr"/>
+      <c r="BR1" t="inlineStr"/>
+      <c r="BS1" t="inlineStr"/>
+      <c r="BT1" t="inlineStr"/>
+      <c r="BU1" t="inlineStr"/>
+      <c r="BV1" t="inlineStr"/>
+      <c r="BW1" t="inlineStr"/>
+      <c r="BX1" t="inlineStr"/>
+      <c r="BY1" t="inlineStr"/>
+      <c r="BZ1" t="inlineStr"/>
+      <c r="CA1" t="inlineStr"/>
+      <c r="CB1" t="inlineStr"/>
+      <c r="CC1" t="inlineStr"/>
+      <c r="CD1" t="inlineStr"/>
+      <c r="CE1" t="inlineStr"/>
+      <c r="CF1" t="inlineStr"/>
+      <c r="CG1" t="inlineStr"/>
+      <c r="CH1" t="inlineStr"/>
+      <c r="CI1" t="inlineStr"/>
+      <c r="CJ1" t="inlineStr"/>
+      <c r="CK1" t="inlineStr"/>
+      <c r="CL1" t="inlineStr"/>
+      <c r="CM1" t="inlineStr"/>
+      <c r="CN1" t="inlineStr"/>
+      <c r="CO1" t="inlineStr"/>
+      <c r="CP1" t="inlineStr"/>
+      <c r="CQ1" t="inlineStr"/>
+      <c r="CR1" t="inlineStr"/>
+      <c r="CS1" t="inlineStr"/>
+      <c r="CT1" t="inlineStr"/>
+      <c r="CU1" t="inlineStr"/>
+      <c r="CV1" t="inlineStr"/>
+      <c r="CW1" t="inlineStr"/>
+      <c r="CX1" t="inlineStr"/>
+      <c r="CY1" t="inlineStr"/>
+      <c r="CZ1" t="inlineStr"/>
+      <c r="DA1" t="inlineStr"/>
+      <c r="DB1" t="inlineStr"/>
+      <c r="DC1" t="inlineStr"/>
+      <c r="DD1" t="inlineStr"/>
+      <c r="DE1" t="inlineStr"/>
+      <c r="DF1" t="inlineStr"/>
+      <c r="DG1" t="inlineStr"/>
+      <c r="DH1" t="inlineStr"/>
+      <c r="DI1" t="inlineStr"/>
+      <c r="DJ1" t="inlineStr"/>
+      <c r="DK1" t="inlineStr"/>
+      <c r="DL1" t="inlineStr"/>
+      <c r="DM1" t="inlineStr"/>
+      <c r="DN1" t="inlineStr"/>
+      <c r="DO1" t="inlineStr"/>
+      <c r="DP1" t="inlineStr"/>
+      <c r="DQ1" t="inlineStr"/>
+      <c r="DR1" t="inlineStr"/>
+      <c r="DS1" t="inlineStr"/>
+      <c r="DT1" t="inlineStr"/>
+      <c r="DU1" t="inlineStr"/>
+      <c r="DV1" t="inlineStr"/>
+      <c r="DW1" t="inlineStr"/>
+      <c r="DX1" t="inlineStr"/>
+      <c r="DY1" t="inlineStr"/>
+      <c r="DZ1" t="inlineStr"/>
+      <c r="EA1" t="inlineStr"/>
+      <c r="EB1" t="inlineStr"/>
+      <c r="EC1" t="inlineStr"/>
+      <c r="ED1" t="inlineStr"/>
+      <c r="EE1" t="inlineStr"/>
+      <c r="EF1" t="inlineStr"/>
+      <c r="EG1" t="inlineStr"/>
+      <c r="EH1" t="inlineStr"/>
+      <c r="EI1" t="inlineStr"/>
+      <c r="EJ1" t="inlineStr"/>
+      <c r="EK1" t="inlineStr"/>
+      <c r="EL1" t="inlineStr"/>
+      <c r="EM1" t="inlineStr"/>
+      <c r="EN1" t="inlineStr"/>
+      <c r="EO1" t="inlineStr"/>
+      <c r="EP1" t="inlineStr"/>
+      <c r="EQ1" t="inlineStr"/>
+      <c r="ER1" t="inlineStr"/>
+      <c r="ES1" t="inlineStr"/>
+      <c r="ET1" t="inlineStr"/>
+      <c r="EU1" t="inlineStr"/>
+      <c r="EV1" t="inlineStr"/>
+      <c r="EW1" t="inlineStr"/>
+      <c r="EX1" t="inlineStr"/>
+      <c r="EY1" t="inlineStr"/>
+      <c r="EZ1" t="inlineStr"/>
+      <c r="FA1" t="inlineStr"/>
+      <c r="FB1" t="inlineStr"/>
+      <c r="FC1" t="inlineStr"/>
+      <c r="FD1" t="inlineStr"/>
+      <c r="FE1" t="inlineStr"/>
+      <c r="FF1" t="inlineStr"/>
+      <c r="FG1" t="inlineStr"/>
+      <c r="FH1" t="inlineStr"/>
+      <c r="FI1" t="inlineStr"/>
+      <c r="FJ1" t="inlineStr"/>
+      <c r="FK1" t="inlineStr"/>
+      <c r="FL1" t="inlineStr"/>
+      <c r="FM1" t="inlineStr"/>
+      <c r="FN1" t="inlineStr"/>
+      <c r="FO1" t="inlineStr"/>
+      <c r="FP1" t="inlineStr"/>
+      <c r="FQ1" t="inlineStr"/>
+      <c r="FR1" t="inlineStr"/>
+      <c r="FS1" t="inlineStr"/>
+      <c r="FT1" t="inlineStr"/>
+      <c r="FU1" t="inlineStr"/>
+      <c r="FV1" t="inlineStr"/>
+      <c r="FW1" t="inlineStr"/>
+      <c r="FX1" t="inlineStr"/>
+      <c r="FY1" t="inlineStr"/>
+      <c r="FZ1" t="inlineStr"/>
+      <c r="GA1" t="inlineStr"/>
+      <c r="GB1" t="inlineStr"/>
+      <c r="GC1" t="inlineStr"/>
+      <c r="GD1" t="inlineStr"/>
+      <c r="GE1" t="inlineStr"/>
+      <c r="GF1" t="inlineStr"/>
+      <c r="GG1" t="inlineStr"/>
+      <c r="GH1" t="inlineStr"/>
+      <c r="GI1" t="inlineStr"/>
+      <c r="GJ1" t="inlineStr"/>
+      <c r="GK1" t="inlineStr"/>
+      <c r="GL1" t="inlineStr"/>
+      <c r="GM1" t="inlineStr"/>
+      <c r="GN1" t="inlineStr"/>
+      <c r="GO1" t="inlineStr"/>
+      <c r="GP1" t="inlineStr"/>
+      <c r="GQ1" t="inlineStr"/>
+      <c r="GR1" t="inlineStr"/>
+      <c r="GS1" t="inlineStr"/>
+      <c r="GT1" t="inlineStr"/>
+      <c r="GU1" t="inlineStr"/>
+      <c r="GV1" t="inlineStr"/>
+      <c r="GW1" t="inlineStr"/>
+      <c r="GX1" t="inlineStr"/>
+      <c r="GY1" t="inlineStr"/>
+      <c r="GZ1" t="inlineStr"/>
+      <c r="HA1" t="inlineStr"/>
+      <c r="HB1" t="inlineStr"/>
+      <c r="HC1" t="inlineStr"/>
+      <c r="HD1" t="inlineStr"/>
+      <c r="HE1" t="inlineStr"/>
+      <c r="HF1" t="inlineStr"/>
+      <c r="HG1" t="inlineStr"/>
+      <c r="HH1" t="inlineStr"/>
+      <c r="HI1" t="inlineStr"/>
+      <c r="HJ1" t="inlineStr"/>
+      <c r="HK1" t="inlineStr"/>
+      <c r="HL1" t="inlineStr"/>
+      <c r="HM1" t="inlineStr"/>
+      <c r="HN1" t="inlineStr"/>
+      <c r="HO1" t="inlineStr"/>
+      <c r="HP1" t="inlineStr"/>
+      <c r="HQ1" t="inlineStr"/>
+      <c r="HR1" t="inlineStr"/>
+      <c r="HS1" t="inlineStr"/>
+      <c r="HT1" t="inlineStr"/>
+      <c r="HU1" t="inlineStr"/>
+      <c r="HV1" t="inlineStr"/>
+      <c r="HW1" t="inlineStr"/>
+      <c r="HX1" t="inlineStr"/>
+      <c r="HY1" t="inlineStr"/>
+      <c r="HZ1" t="inlineStr"/>
+      <c r="IA1" t="inlineStr"/>
+      <c r="IB1" t="inlineStr"/>
+      <c r="IC1" t="inlineStr"/>
+      <c r="ID1" t="inlineStr"/>
+      <c r="IE1" t="inlineStr"/>
+      <c r="IF1" t="inlineStr"/>
+      <c r="IG1" t="inlineStr"/>
+      <c r="IH1" t="inlineStr"/>
+      <c r="II1" t="inlineStr"/>
+      <c r="IJ1" t="inlineStr"/>
+      <c r="IK1" t="inlineStr"/>
+      <c r="IL1" t="inlineStr"/>
+      <c r="IM1" t="inlineStr"/>
+      <c r="IN1" t="inlineStr"/>
+      <c r="IO1" t="inlineStr"/>
+      <c r="IP1" t="inlineStr"/>
+      <c r="IQ1" t="inlineStr"/>
+      <c r="IR1" t="inlineStr"/>
+      <c r="IS1" t="inlineStr"/>
+      <c r="IT1" t="inlineStr"/>
+      <c r="IU1" t="inlineStr"/>
+      <c r="IV1" t="inlineStr"/>
+      <c r="IW1" t="inlineStr"/>
+      <c r="IX1" t="inlineStr"/>
+      <c r="IY1" t="inlineStr"/>
+      <c r="IZ1" t="inlineStr"/>
+      <c r="JA1" t="inlineStr"/>
+      <c r="JB1" t="inlineStr"/>
+      <c r="JC1" t="inlineStr"/>
+      <c r="JD1" t="inlineStr"/>
+      <c r="JE1" t="inlineStr"/>
+      <c r="JF1" t="inlineStr"/>
+      <c r="JG1" t="inlineStr"/>
+      <c r="JH1" t="inlineStr"/>
+      <c r="JI1" t="inlineStr"/>
+      <c r="JJ1" t="inlineStr"/>
+      <c r="JK1" t="inlineStr"/>
+      <c r="JL1" t="inlineStr"/>
+      <c r="JM1" t="inlineStr"/>
+      <c r="JN1" t="inlineStr"/>
+      <c r="JO1" t="inlineStr"/>
+      <c r="JP1" t="inlineStr"/>
+      <c r="JQ1" t="inlineStr"/>
+      <c r="JR1" t="inlineStr"/>
+      <c r="JS1" t="inlineStr"/>
+      <c r="JT1" t="inlineStr"/>
+      <c r="JU1" t="inlineStr"/>
+      <c r="JV1" t="inlineStr"/>
+      <c r="JW1" t="inlineStr"/>
+      <c r="JX1" t="inlineStr"/>
+      <c r="JY1" t="inlineStr"/>
+      <c r="JZ1" t="inlineStr"/>
+      <c r="KA1" t="inlineStr"/>
+      <c r="KB1" t="inlineStr"/>
+      <c r="KC1" t="inlineStr"/>
+      <c r="KD1" t="inlineStr"/>
+      <c r="KE1" t="inlineStr"/>
+      <c r="KF1" t="inlineStr"/>
+      <c r="KG1" t="inlineStr"/>
+      <c r="KH1" t="inlineStr"/>
+      <c r="KI1" t="inlineStr"/>
+      <c r="KJ1" t="inlineStr"/>
+      <c r="KK1" t="inlineStr"/>
+      <c r="KL1" t="inlineStr"/>
+      <c r="KM1" t="inlineStr"/>
+      <c r="KN1" t="inlineStr"/>
+      <c r="KO1" t="inlineStr"/>
+      <c r="KP1" t="inlineStr"/>
+      <c r="KQ1" t="inlineStr"/>
+      <c r="KR1" t="inlineStr"/>
+      <c r="KS1" t="inlineStr"/>
+      <c r="KT1" t="inlineStr"/>
+      <c r="KU1" t="inlineStr"/>
+      <c r="KV1" t="inlineStr"/>
+      <c r="KW1" t="inlineStr"/>
+      <c r="KX1" t="inlineStr"/>
+      <c r="KY1" t="inlineStr"/>
+      <c r="KZ1" t="inlineStr"/>
+      <c r="LA1" t="inlineStr"/>
+      <c r="LB1" t="inlineStr"/>
+      <c r="LC1" t="inlineStr"/>
+      <c r="LD1" t="inlineStr"/>
+      <c r="LE1" t="inlineStr"/>
+      <c r="LF1" t="inlineStr"/>
+      <c r="LG1" t="inlineStr"/>
+      <c r="LH1" t="inlineStr"/>
+      <c r="LI1" t="inlineStr"/>
+      <c r="LJ1" t="inlineStr"/>
+      <c r="LK1" t="inlineStr"/>
+      <c r="LL1" t="inlineStr"/>
+      <c r="LM1" t="inlineStr"/>
+      <c r="LN1" t="inlineStr"/>
+      <c r="LO1" t="inlineStr"/>
+      <c r="LP1" t="inlineStr"/>
+      <c r="LQ1" t="inlineStr"/>
+      <c r="LR1" t="inlineStr"/>
+      <c r="LS1" t="inlineStr"/>
+      <c r="LT1" t="inlineStr"/>
+      <c r="LU1" t="inlineStr"/>
+      <c r="LV1" t="inlineStr"/>
+      <c r="LW1" t="inlineStr"/>
+      <c r="LX1" t="inlineStr"/>
+      <c r="LY1" t="inlineStr"/>
+      <c r="LZ1" t="inlineStr"/>
+      <c r="MA1" t="inlineStr"/>
+      <c r="MB1" t="inlineStr"/>
+      <c r="MC1" t="inlineStr"/>
+      <c r="MD1" t="inlineStr"/>
+      <c r="ME1" t="inlineStr"/>
+      <c r="MF1" t="inlineStr"/>
+      <c r="MG1" t="inlineStr"/>
+      <c r="MH1" t="inlineStr"/>
+      <c r="MI1" t="inlineStr"/>
+      <c r="MJ1" t="inlineStr"/>
+      <c r="MK1" t="inlineStr"/>
+      <c r="ML1" t="inlineStr"/>
+      <c r="MM1" t="inlineStr"/>
+      <c r="MN1" t="inlineStr"/>
+      <c r="MO1" t="inlineStr"/>
+      <c r="MP1" t="inlineStr"/>
+      <c r="MQ1" t="inlineStr"/>
+      <c r="MR1" t="inlineStr"/>
+      <c r="MS1" t="inlineStr"/>
+      <c r="MT1" t="inlineStr"/>
+      <c r="MU1" t="inlineStr"/>
+      <c r="MV1" t="inlineStr"/>
+      <c r="MW1" t="inlineStr"/>
+      <c r="MX1" t="inlineStr"/>
+      <c r="MY1" t="inlineStr"/>
+      <c r="MZ1" t="inlineStr"/>
+      <c r="NA1" t="inlineStr"/>
+      <c r="NB1" t="inlineStr"/>
+      <c r="NC1" t="inlineStr"/>
+      <c r="ND1" t="inlineStr"/>
+      <c r="NE1" t="inlineStr"/>
+      <c r="NF1" t="inlineStr"/>
+      <c r="NG1" t="inlineStr"/>
+      <c r="NH1" t="inlineStr"/>
+      <c r="NI1" t="inlineStr"/>
+      <c r="NJ1" t="inlineStr"/>
+      <c r="NK1" t="inlineStr"/>
+      <c r="NL1" t="inlineStr"/>
+      <c r="NM1" t="inlineStr"/>
+      <c r="NN1" t="inlineStr"/>
+      <c r="NO1" t="inlineStr"/>
+      <c r="NP1" t="inlineStr"/>
+      <c r="NQ1" t="inlineStr"/>
+      <c r="NR1" t="inlineStr"/>
+      <c r="NS1" t="inlineStr"/>
+      <c r="NT1" t="inlineStr"/>
+      <c r="NU1" t="inlineStr"/>
+      <c r="NV1" t="inlineStr"/>
+      <c r="NW1" t="inlineStr"/>
+      <c r="NX1" t="inlineStr"/>
+      <c r="NY1" t="inlineStr"/>
+      <c r="NZ1" t="inlineStr"/>
+      <c r="OA1" t="inlineStr"/>
+      <c r="OB1" t="inlineStr"/>
+      <c r="OC1" t="inlineStr"/>
+      <c r="OD1" t="inlineStr"/>
+      <c r="OE1" t="inlineStr"/>
+      <c r="OF1" t="inlineStr"/>
+      <c r="OG1" t="inlineStr"/>
+      <c r="OH1" t="inlineStr"/>
+      <c r="OI1" t="inlineStr"/>
+      <c r="OJ1" t="inlineStr"/>
+      <c r="OK1" t="inlineStr"/>
+      <c r="OL1" t="inlineStr"/>
+      <c r="OM1" t="inlineStr"/>
+      <c r="ON1" t="inlineStr"/>
+      <c r="OO1" t="inlineStr"/>
+      <c r="OP1" t="inlineStr"/>
+      <c r="OQ1" t="inlineStr"/>
+      <c r="OR1" t="inlineStr"/>
+      <c r="OS1" t="inlineStr"/>
+      <c r="OT1" t="inlineStr"/>
+      <c r="OU1" t="inlineStr"/>
+      <c r="OV1" t="inlineStr"/>
+      <c r="OW1" t="inlineStr"/>
+      <c r="OX1" t="inlineStr"/>
+      <c r="OY1" t="inlineStr"/>
+      <c r="OZ1" t="inlineStr"/>
+      <c r="PA1" t="inlineStr"/>
+      <c r="PB1" t="inlineStr"/>
+      <c r="PC1" t="inlineStr"/>
+      <c r="PD1" t="inlineStr"/>
+      <c r="PE1" t="inlineStr"/>
+      <c r="PF1" t="inlineStr"/>
+      <c r="PG1" t="inlineStr"/>
+      <c r="PH1" t="inlineStr"/>
+      <c r="PI1" t="inlineStr"/>
+      <c r="PJ1" t="inlineStr"/>
+      <c r="PK1" t="inlineStr"/>
+      <c r="PL1" t="inlineStr"/>
+      <c r="PM1" t="inlineStr"/>
+      <c r="PN1" t="inlineStr"/>
+      <c r="PO1" t="inlineStr"/>
+      <c r="PP1" t="inlineStr"/>
+      <c r="PQ1" t="inlineStr"/>
+      <c r="PR1" t="inlineStr"/>
+      <c r="PS1" t="inlineStr"/>
+      <c r="PT1" t="inlineStr"/>
+      <c r="PU1" t="inlineStr"/>
+      <c r="PV1" t="inlineStr"/>
+      <c r="PW1" t="inlineStr"/>
+      <c r="PX1" t="inlineStr"/>
+      <c r="PY1" t="inlineStr"/>
+      <c r="PZ1" t="inlineStr"/>
+      <c r="QA1" t="inlineStr"/>
+      <c r="QB1" t="inlineStr"/>
+      <c r="QC1" t="inlineStr"/>
+      <c r="QD1" t="inlineStr"/>
+      <c r="QE1" t="inlineStr"/>
+      <c r="QF1" t="inlineStr"/>
+      <c r="QG1" t="inlineStr"/>
+      <c r="QH1" t="inlineStr"/>
+      <c r="QI1" t="inlineStr"/>
+      <c r="QJ1" t="inlineStr"/>
+      <c r="QK1" t="inlineStr"/>
+      <c r="QL1" t="inlineStr"/>
+      <c r="QM1" t="inlineStr"/>
+      <c r="QN1" t="inlineStr"/>
+      <c r="QO1" t="inlineStr"/>
+      <c r="QP1" t="inlineStr"/>
+      <c r="QQ1" t="inlineStr"/>
+      <c r="QR1" t="inlineStr"/>
+      <c r="QS1" t="inlineStr"/>
+      <c r="QT1" t="inlineStr"/>
+      <c r="QU1" t="inlineStr"/>
+      <c r="QV1" t="inlineStr"/>
+      <c r="QW1" t="inlineStr"/>
+      <c r="QX1" t="inlineStr"/>
+      <c r="QY1" t="inlineStr"/>
+      <c r="QZ1" t="inlineStr"/>
+      <c r="RA1" t="inlineStr"/>
+      <c r="RB1" t="inlineStr"/>
+      <c r="RC1" t="inlineStr"/>
+      <c r="RD1" t="inlineStr"/>
+      <c r="RE1" t="inlineStr"/>
+      <c r="RF1" t="inlineStr"/>
+      <c r="RG1" t="inlineStr"/>
+      <c r="RH1" t="inlineStr"/>
+      <c r="RI1" t="inlineStr"/>
+      <c r="RJ1" t="inlineStr"/>
+      <c r="RK1" t="inlineStr"/>
+      <c r="RL1" t="inlineStr"/>
+      <c r="RM1" t="inlineStr"/>
+      <c r="RN1" t="inlineStr"/>
+      <c r="RO1" t="inlineStr"/>
+      <c r="RP1" t="inlineStr"/>
+      <c r="RQ1" t="inlineStr"/>
+      <c r="RR1" t="inlineStr"/>
+      <c r="RS1" t="inlineStr"/>
+      <c r="RT1" t="inlineStr"/>
+      <c r="RU1" t="inlineStr"/>
+      <c r="RV1" t="inlineStr"/>
+      <c r="RW1" t="inlineStr"/>
+      <c r="RX1" t="inlineStr"/>
+      <c r="RY1" t="inlineStr"/>
+      <c r="RZ1" t="inlineStr"/>
+      <c r="SA1" t="inlineStr"/>
+      <c r="SB1" t="inlineStr"/>
+      <c r="SC1" t="inlineStr"/>
+      <c r="SD1" t="inlineStr"/>
+      <c r="SE1" t="inlineStr"/>
+      <c r="SF1" t="inlineStr"/>
+      <c r="SG1" t="inlineStr"/>
+      <c r="SH1" t="inlineStr"/>
+      <c r="SI1" t="inlineStr"/>
+      <c r="SJ1" t="inlineStr"/>
+      <c r="SK1" t="inlineStr"/>
+      <c r="SL1" t="inlineStr"/>
+      <c r="SM1" t="inlineStr"/>
+      <c r="SN1" t="inlineStr"/>
+      <c r="SO1" t="inlineStr"/>
+      <c r="SP1" t="inlineStr"/>
+      <c r="SQ1" t="inlineStr"/>
+      <c r="SR1" t="inlineStr"/>
+      <c r="SS1" t="inlineStr"/>
+      <c r="ST1" t="inlineStr"/>
+      <c r="SU1" t="inlineStr"/>
+      <c r="SV1" t="inlineStr"/>
+      <c r="SW1" t="inlineStr"/>
+      <c r="SX1" t="inlineStr"/>
+      <c r="SY1" t="inlineStr"/>
+      <c r="SZ1" t="inlineStr"/>
+      <c r="TA1" t="inlineStr"/>
+      <c r="TB1" t="inlineStr"/>
+      <c r="TC1" t="inlineStr"/>
+      <c r="TD1" t="inlineStr"/>
+      <c r="TE1" t="inlineStr"/>
+      <c r="TF1" t="inlineStr"/>
+      <c r="TG1" t="inlineStr"/>
+      <c r="TH1" t="inlineStr"/>
+      <c r="TI1" t="inlineStr"/>
+      <c r="TJ1" t="inlineStr"/>
+      <c r="TK1" t="inlineStr"/>
+      <c r="TL1" t="inlineStr"/>
+      <c r="TM1" t="inlineStr"/>
+      <c r="TN1" t="inlineStr"/>
+      <c r="TO1" t="inlineStr"/>
+      <c r="TP1" t="inlineStr"/>
+      <c r="TQ1" t="inlineStr"/>
+      <c r="TR1" t="inlineStr"/>
+      <c r="TS1" t="inlineStr"/>
+      <c r="TT1" t="inlineStr"/>
+      <c r="TU1" t="inlineStr"/>
+      <c r="TV1" t="inlineStr"/>
+      <c r="TW1" t="inlineStr"/>
+      <c r="TX1" t="inlineStr"/>
+      <c r="TY1" t="inlineStr"/>
+      <c r="TZ1" t="inlineStr"/>
+      <c r="UA1" t="inlineStr"/>
+      <c r="UB1" t="inlineStr"/>
+      <c r="UC1" t="inlineStr"/>
+      <c r="UD1" t="inlineStr"/>
+      <c r="UE1" t="inlineStr"/>
+      <c r="UF1" t="inlineStr"/>
+      <c r="UG1" t="inlineStr"/>
+      <c r="UH1" t="inlineStr"/>
+      <c r="UI1" t="inlineStr"/>
+      <c r="UJ1" t="inlineStr"/>
+      <c r="UK1" t="inlineStr"/>
+      <c r="UL1" t="inlineStr"/>
+      <c r="UM1" t="inlineStr"/>
+      <c r="UN1" t="inlineStr"/>
+      <c r="UO1" t="inlineStr"/>
+      <c r="UP1" t="inlineStr"/>
+      <c r="UQ1" t="inlineStr"/>
+      <c r="UR1" t="inlineStr"/>
+      <c r="US1" t="inlineStr"/>
+      <c r="UT1" t="inlineStr"/>
+      <c r="UU1" t="inlineStr"/>
+      <c r="UV1" t="inlineStr"/>
+      <c r="UW1" t="inlineStr"/>
+      <c r="UX1" t="inlineStr"/>
+      <c r="UY1" t="inlineStr"/>
+      <c r="UZ1" t="inlineStr"/>
+      <c r="VA1" t="inlineStr"/>
+      <c r="VB1" t="inlineStr"/>
+      <c r="VC1" t="inlineStr"/>
+      <c r="VD1" t="inlineStr"/>
+      <c r="VE1" t="inlineStr"/>
+      <c r="VF1" t="inlineStr"/>
+      <c r="VG1" t="inlineStr"/>
+      <c r="VH1" t="inlineStr"/>
+      <c r="VI1" t="inlineStr"/>
+      <c r="VJ1" t="inlineStr"/>
+      <c r="VK1" t="inlineStr"/>
+      <c r="VL1" t="inlineStr"/>
+      <c r="VM1" t="inlineStr"/>
+      <c r="VN1" t="inlineStr"/>
+      <c r="VO1" t="inlineStr"/>
+      <c r="VP1" t="inlineStr"/>
+      <c r="VQ1" t="inlineStr"/>
+      <c r="VR1" t="inlineStr"/>
+      <c r="VS1" t="inlineStr"/>
+      <c r="VT1" t="inlineStr"/>
+      <c r="VU1" t="inlineStr"/>
+      <c r="VV1" t="inlineStr"/>
+      <c r="VW1" t="inlineStr"/>
+      <c r="VX1" t="inlineStr"/>
+      <c r="VY1" t="inlineStr"/>
+      <c r="VZ1" t="inlineStr"/>
+      <c r="WA1" t="inlineStr"/>
+      <c r="WB1" t="inlineStr"/>
+      <c r="WC1" t="inlineStr"/>
+      <c r="WD1" t="inlineStr"/>
+      <c r="WE1" t="inlineStr"/>
+      <c r="WF1" t="inlineStr"/>
+      <c r="WG1" t="inlineStr"/>
+      <c r="WH1" t="inlineStr"/>
+      <c r="WI1" t="inlineStr"/>
+      <c r="WJ1" t="inlineStr"/>
+      <c r="WK1" t="inlineStr"/>
+      <c r="WL1" t="inlineStr"/>
+      <c r="WM1" t="inlineStr"/>
+      <c r="WN1" t="inlineStr"/>
+      <c r="WO1" t="inlineStr"/>
+      <c r="WP1" t="inlineStr"/>
+      <c r="WQ1" t="inlineStr"/>
+      <c r="WR1" t="inlineStr"/>
+      <c r="WS1" t="inlineStr"/>
+      <c r="WT1" t="inlineStr"/>
+      <c r="WU1" t="inlineStr"/>
+      <c r="WV1" t="inlineStr"/>
+      <c r="WW1" t="inlineStr"/>
+      <c r="WX1" t="inlineStr"/>
+      <c r="WY1" t="inlineStr"/>
+      <c r="WZ1" t="inlineStr"/>
+      <c r="XA1" t="inlineStr"/>
+      <c r="XB1" t="inlineStr"/>
+      <c r="XC1" t="inlineStr"/>
+      <c r="XD1" t="inlineStr"/>
+      <c r="XE1" t="inlineStr"/>
+      <c r="XF1" t="inlineStr"/>
+      <c r="XG1" t="inlineStr"/>
+      <c r="XH1" t="inlineStr"/>
+      <c r="XI1" t="inlineStr"/>
+      <c r="XJ1" t="inlineStr"/>
+      <c r="XK1" t="inlineStr"/>
+      <c r="XL1" t="inlineStr"/>
+      <c r="XM1" t="inlineStr"/>
+      <c r="XN1" t="inlineStr"/>
+      <c r="XO1" t="inlineStr"/>
+      <c r="XP1" t="inlineStr"/>
+      <c r="XQ1" t="inlineStr"/>
+      <c r="XR1" t="inlineStr"/>
+      <c r="XS1" t="inlineStr"/>
+      <c r="XT1" t="inlineStr"/>
+      <c r="XU1" t="inlineStr"/>
+      <c r="XV1" t="inlineStr"/>
+      <c r="XW1" t="inlineStr"/>
+      <c r="XX1" t="inlineStr"/>
+      <c r="XY1" t="inlineStr"/>
+      <c r="XZ1" t="inlineStr"/>
+      <c r="YA1" t="inlineStr"/>
+      <c r="YB1" t="inlineStr"/>
+      <c r="YC1" t="inlineStr"/>
+      <c r="YD1" t="inlineStr"/>
+      <c r="YE1" t="inlineStr"/>
+      <c r="YF1" t="inlineStr"/>
+      <c r="YG1" t="inlineStr"/>
+      <c r="YH1" t="inlineStr"/>
+      <c r="YI1" t="inlineStr"/>
+      <c r="YJ1" t="inlineStr"/>
+      <c r="YK1" t="inlineStr"/>
+      <c r="YL1" t="inlineStr"/>
+      <c r="YM1" t="inlineStr"/>
+      <c r="YN1" t="inlineStr"/>
+      <c r="YO1" t="inlineStr"/>
+      <c r="YP1" t="inlineStr"/>
+      <c r="YQ1" t="inlineStr"/>
+      <c r="YR1" t="inlineStr"/>
+      <c r="YS1" t="inlineStr"/>
+      <c r="YT1" t="inlineStr"/>
+      <c r="YU1" t="inlineStr"/>
+      <c r="YV1" t="inlineStr"/>
+      <c r="YW1" t="inlineStr"/>
+      <c r="YX1" t="inlineStr"/>
+      <c r="YY1" t="inlineStr"/>
+      <c r="YZ1" t="inlineStr"/>
+      <c r="ZA1" t="inlineStr"/>
+      <c r="ZB1" t="inlineStr"/>
+      <c r="ZC1" t="inlineStr"/>
+      <c r="ZD1" t="inlineStr"/>
+      <c r="ZE1" t="inlineStr"/>
+      <c r="ZF1" t="inlineStr"/>
+      <c r="ZG1" t="inlineStr"/>
+      <c r="ZH1" t="inlineStr"/>
+      <c r="ZI1" t="inlineStr"/>
+      <c r="ZJ1" t="inlineStr"/>
+      <c r="ZK1" t="inlineStr"/>
+      <c r="ZL1" t="inlineStr"/>
+      <c r="ZM1" t="inlineStr"/>
+      <c r="ZN1" t="inlineStr"/>
+      <c r="ZO1" t="inlineStr"/>
+      <c r="ZP1" t="inlineStr"/>
+      <c r="ZQ1" t="inlineStr"/>
+      <c r="ZR1" t="inlineStr"/>
+      <c r="ZS1" t="inlineStr"/>
+      <c r="ZT1" t="inlineStr"/>
+      <c r="ZU1" t="inlineStr"/>
+      <c r="ZV1" t="inlineStr"/>
+      <c r="ZW1" t="inlineStr"/>
+      <c r="ZX1" t="inlineStr"/>
+      <c r="ZY1" t="inlineStr"/>
+      <c r="ZZ1" t="inlineStr"/>
+      <c r="AAA1" t="inlineStr"/>
+      <c r="AAB1" t="inlineStr"/>
+      <c r="AAC1" t="inlineStr"/>
+      <c r="AAD1" t="inlineStr"/>
+      <c r="AAE1" t="inlineStr"/>
+      <c r="AAF1" t="inlineStr"/>
+      <c r="AAG1" t="inlineStr"/>
+      <c r="AAH1" t="inlineStr"/>
+      <c r="AAI1" t="inlineStr"/>
+      <c r="AAJ1" t="inlineStr"/>
+      <c r="AAK1" t="inlineStr"/>
+      <c r="AAL1" t="inlineStr"/>
+      <c r="AAM1" t="inlineStr"/>
+      <c r="AAN1" t="inlineStr"/>
+      <c r="AAO1" t="inlineStr"/>
+      <c r="AAP1" t="inlineStr"/>
+      <c r="AAQ1" t="inlineStr"/>
+      <c r="AAR1" t="inlineStr"/>
+      <c r="AAS1" t="inlineStr"/>
+      <c r="AAT1" t="inlineStr"/>
+      <c r="AAU1" t="inlineStr"/>
+      <c r="AAV1" t="inlineStr"/>
+      <c r="AAW1" t="inlineStr"/>
+      <c r="AAX1" t="inlineStr"/>
+      <c r="AAY1" t="inlineStr"/>
+      <c r="AAZ1" t="inlineStr"/>
+      <c r="ABA1" t="inlineStr"/>
+      <c r="ABB1" t="inlineStr"/>
+      <c r="ABC1" t="inlineStr"/>
+      <c r="ABD1" t="inlineStr"/>
+      <c r="ABE1" t="inlineStr"/>
+      <c r="ABF1" t="inlineStr"/>
+      <c r="ABG1" t="inlineStr"/>
+      <c r="ABH1" t="inlineStr"/>
+      <c r="ABI1" t="inlineStr"/>
+      <c r="ABJ1" t="inlineStr"/>
+      <c r="ABK1" t="inlineStr"/>
+      <c r="ABL1" t="inlineStr"/>
+      <c r="ABM1" t="inlineStr"/>
+      <c r="ABN1" t="inlineStr"/>
+      <c r="ABO1" t="inlineStr"/>
+      <c r="ABP1" t="inlineStr"/>
+      <c r="ABQ1" t="inlineStr"/>
+      <c r="ABR1" t="inlineStr"/>
+      <c r="ABS1" t="inlineStr"/>
+      <c r="ABT1" t="inlineStr"/>
+      <c r="ABU1" t="inlineStr"/>
+      <c r="ABV1" t="inlineStr"/>
+      <c r="ABW1" t="inlineStr"/>
+      <c r="ABX1" t="inlineStr"/>
+      <c r="ABY1" t="inlineStr"/>
+      <c r="ABZ1" t="inlineStr"/>
+      <c r="ACA1" t="inlineStr"/>
+      <c r="ACB1" t="inlineStr"/>
+      <c r="ACC1" t="inlineStr"/>
+      <c r="ACD1" t="inlineStr"/>
+      <c r="ACE1" t="inlineStr"/>
+      <c r="ACF1" t="inlineStr"/>
+      <c r="ACG1" t="inlineStr"/>
+      <c r="ACH1" t="inlineStr"/>
+      <c r="ACI1" t="inlineStr"/>
+      <c r="ACJ1" t="inlineStr"/>
+      <c r="ACK1" t="inlineStr"/>
+      <c r="ACL1" t="inlineStr"/>
+      <c r="ACM1" t="inlineStr"/>
+      <c r="ACN1" t="inlineStr"/>
+      <c r="ACO1" t="inlineStr"/>
+      <c r="ACP1" t="inlineStr"/>
+      <c r="ACQ1" t="inlineStr"/>
+      <c r="ACR1" t="inlineStr"/>
+      <c r="ACS1" t="inlineStr"/>
+      <c r="ACT1" t="inlineStr"/>
+      <c r="ACU1" t="inlineStr"/>
+      <c r="ACV1" t="inlineStr"/>
+      <c r="ACW1" t="inlineStr"/>
+      <c r="ACX1" t="inlineStr"/>
+      <c r="ACY1" t="inlineStr"/>
+      <c r="ACZ1" t="inlineStr"/>
+      <c r="ADA1" t="inlineStr"/>
+      <c r="ADB1" t="inlineStr"/>
+      <c r="ADC1" t="inlineStr"/>
+      <c r="ADD1" t="inlineStr"/>
+      <c r="ADE1" t="inlineStr"/>
+      <c r="ADF1" t="inlineStr"/>
+      <c r="ADG1" t="inlineStr"/>
+      <c r="ADH1" t="inlineStr"/>
+      <c r="ADI1" t="inlineStr"/>
+      <c r="ADJ1" t="inlineStr"/>
+      <c r="ADK1" t="inlineStr"/>
+      <c r="ADL1" t="inlineStr"/>
+      <c r="ADM1" t="inlineStr"/>
+      <c r="ADN1" t="inlineStr"/>
+      <c r="ADO1" t="inlineStr"/>
+      <c r="ADP1" t="inlineStr"/>
+      <c r="ADQ1" t="inlineStr"/>
+      <c r="ADR1" t="inlineStr"/>
+      <c r="ADS1" t="inlineStr"/>
+      <c r="ADT1" t="inlineStr"/>
+      <c r="ADU1" t="inlineStr"/>
+      <c r="ADV1" t="inlineStr"/>
+      <c r="ADW1" t="inlineStr"/>
+      <c r="ADX1" t="inlineStr"/>
+      <c r="ADY1" t="inlineStr"/>
+      <c r="ADZ1" t="inlineStr"/>
+      <c r="AEA1" t="inlineStr"/>
+      <c r="AEB1" t="inlineStr"/>
+      <c r="AEC1" t="inlineStr"/>
+      <c r="AED1" t="inlineStr"/>
+      <c r="AEE1" t="inlineStr"/>
+      <c r="AEF1" t="inlineStr"/>
+      <c r="AEG1" t="inlineStr"/>
+      <c r="AEH1" t="inlineStr"/>
+      <c r="AEI1" t="inlineStr"/>
+      <c r="AEJ1" t="inlineStr"/>
+      <c r="AEK1" t="inlineStr"/>
+      <c r="AEL1" t="inlineStr"/>
+      <c r="AEM1" t="inlineStr"/>
+      <c r="AEN1" t="inlineStr"/>
+      <c r="AEO1" t="inlineStr"/>
+      <c r="AEP1" t="inlineStr"/>
+      <c r="AEQ1" t="inlineStr"/>
+      <c r="AER1" t="inlineStr"/>
+      <c r="AES1" t="inlineStr"/>
+      <c r="AET1" t="inlineStr"/>
+      <c r="AEU1" t="inlineStr"/>
+      <c r="AEV1" t="inlineStr"/>
+      <c r="AEW1" t="inlineStr"/>
+      <c r="AEX1" t="inlineStr"/>
+      <c r="AEY1" t="inlineStr"/>
+      <c r="AEZ1" t="inlineStr"/>
+      <c r="AFA1" t="inlineStr"/>
+      <c r="AFB1" t="inlineStr"/>
+      <c r="AFC1" t="inlineStr"/>
+      <c r="AFD1" t="inlineStr"/>
+      <c r="AFE1" t="inlineStr"/>
+      <c r="AFF1" t="inlineStr"/>
+      <c r="AFG1" t="inlineStr"/>
+      <c r="AFH1" t="inlineStr"/>
+      <c r="AFI1" t="inlineStr"/>
+      <c r="AFJ1" t="inlineStr"/>
+      <c r="AFK1" t="inlineStr"/>
+      <c r="AFL1" t="inlineStr"/>
+      <c r="AFM1" t="inlineStr"/>
+      <c r="AFN1" t="inlineStr"/>
+      <c r="AFO1" t="inlineStr"/>
+      <c r="AFP1" t="inlineStr"/>
+      <c r="AFQ1" t="inlineStr"/>
+      <c r="AFR1" t="inlineStr"/>
+      <c r="AFS1" t="inlineStr"/>
+      <c r="AFT1" t="inlineStr"/>
+      <c r="AFU1" t="inlineStr"/>
+      <c r="AFV1" t="inlineStr"/>
+      <c r="AFW1" t="inlineStr"/>
+      <c r="AFX1" t="inlineStr"/>
+      <c r="AFY1" t="inlineStr"/>
+      <c r="AFZ1" t="inlineStr"/>
+      <c r="AGA1" t="inlineStr"/>
+      <c r="AGB1" t="inlineStr"/>
+      <c r="AGC1" t="inlineStr"/>
+      <c r="AGD1" t="inlineStr"/>
+      <c r="AGE1" t="inlineStr"/>
+      <c r="AGF1" t="inlineStr"/>
+      <c r="AGG1" t="inlineStr"/>
+      <c r="AGH1" t="inlineStr"/>
+      <c r="AGI1" t="inlineStr"/>
+      <c r="AGJ1" t="inlineStr"/>
+      <c r="AGK1" t="inlineStr"/>
+      <c r="AGL1" t="inlineStr"/>
+      <c r="AGM1" t="inlineStr"/>
+      <c r="AGN1" t="inlineStr"/>
+      <c r="AGO1" t="inlineStr"/>
+      <c r="AGP1" t="inlineStr"/>
+      <c r="AGQ1" t="inlineStr"/>
+      <c r="AGR1" t="inlineStr"/>
+      <c r="AGS1" t="inlineStr"/>
+      <c r="AGT1" t="inlineStr"/>
+      <c r="AGU1" t="inlineStr"/>
+      <c r="AGV1" t="inlineStr"/>
+      <c r="AGW1" t="inlineStr"/>
+      <c r="AGX1" t="inlineStr"/>
+      <c r="AGY1" t="inlineStr"/>
+      <c r="AGZ1" t="inlineStr"/>
+      <c r="AHA1" t="inlineStr"/>
+      <c r="AHB1" t="inlineStr"/>
+      <c r="AHC1" t="inlineStr"/>
+      <c r="AHD1" t="inlineStr"/>
+      <c r="AHE1" t="inlineStr"/>
+      <c r="AHF1" t="inlineStr"/>
+      <c r="AHG1" t="inlineStr"/>
+      <c r="AHH1" t="inlineStr"/>
+      <c r="AHI1" t="inlineStr"/>
+      <c r="AHJ1" t="inlineStr"/>
+      <c r="AHK1" t="inlineStr"/>
+      <c r="AHL1" t="inlineStr"/>
+      <c r="AHM1" t="inlineStr"/>
+      <c r="AHN1" t="inlineStr"/>
+      <c r="AHO1" t="inlineStr"/>
+      <c r="AHP1" t="inlineStr"/>
+      <c r="AHQ1" t="inlineStr"/>
+      <c r="AHR1" t="inlineStr"/>
+      <c r="AHS1" t="inlineStr"/>
+      <c r="AHT1" t="inlineStr"/>
+      <c r="AHU1" t="inlineStr"/>
+      <c r="AHV1" t="inlineStr"/>
+      <c r="AHW1" t="inlineStr"/>
+      <c r="AHX1" t="inlineStr"/>
+      <c r="AHY1" t="inlineStr"/>
+      <c r="AHZ1" t="inlineStr"/>
+      <c r="AIA1" t="inlineStr"/>
+      <c r="AIB1" t="inlineStr"/>
+      <c r="AIC1" t="inlineStr"/>
+      <c r="AID1" t="inlineStr"/>
+      <c r="AIE1" t="inlineStr"/>
+      <c r="AIF1" t="inlineStr"/>
+      <c r="AIG1" t="inlineStr"/>
+      <c r="AIH1" t="inlineStr"/>
+      <c r="AII1" t="inlineStr"/>
+      <c r="AIJ1" t="inlineStr"/>
+      <c r="AIK1" t="inlineStr"/>
+      <c r="AIL1" t="inlineStr"/>
+      <c r="AIM1" t="inlineStr"/>
+      <c r="AIN1" t="inlineStr"/>
+      <c r="AIO1" t="inlineStr"/>
+      <c r="AIP1" t="inlineStr"/>
+      <c r="AIQ1" t="inlineStr"/>
+      <c r="AIR1" t="inlineStr"/>
+      <c r="AIS1" t="inlineStr"/>
+      <c r="AIT1" t="inlineStr"/>
+      <c r="AIU1" t="inlineStr"/>
+      <c r="AIV1" t="inlineStr"/>
+      <c r="AIW1" t="inlineStr"/>
+      <c r="AIX1" t="inlineStr"/>
+      <c r="AIY1" t="inlineStr"/>
+      <c r="AIZ1" t="inlineStr"/>
+      <c r="AJA1" t="inlineStr"/>
+      <c r="AJB1" t="inlineStr"/>
+      <c r="AJC1" t="inlineStr"/>
+      <c r="AJD1" t="inlineStr"/>
+      <c r="AJE1" t="inlineStr"/>
+      <c r="AJF1" t="inlineStr"/>
+      <c r="AJG1" t="inlineStr"/>
+      <c r="AJH1" t="inlineStr"/>
+      <c r="AJI1" t="inlineStr"/>
+      <c r="AJJ1" t="inlineStr"/>
+      <c r="AJK1" t="inlineStr"/>
+      <c r="AJL1" t="inlineStr"/>
+      <c r="AJM1" t="inlineStr"/>
+      <c r="AJN1" t="inlineStr"/>
+      <c r="AJO1" t="inlineStr"/>
+      <c r="AJP1" t="inlineStr"/>
+      <c r="AJQ1" t="inlineStr"/>
+      <c r="AJR1" t="inlineStr"/>
+      <c r="AJS1" t="inlineStr"/>
+      <c r="AJT1" t="inlineStr"/>
+      <c r="AJU1" t="inlineStr"/>
+      <c r="AJV1" t="inlineStr"/>
+      <c r="AJW1" t="inlineStr"/>
+      <c r="AJX1" t="inlineStr"/>
+      <c r="AJY1" t="inlineStr"/>
+      <c r="AJZ1" t="inlineStr"/>
+      <c r="AKA1" t="inlineStr"/>
+      <c r="AKB1" t="inlineStr"/>
+      <c r="AKC1" t="inlineStr"/>
+      <c r="AKD1" t="inlineStr"/>
+      <c r="AKE1" t="inlineStr"/>
+      <c r="AKF1" t="inlineStr"/>
+      <c r="AKG1" t="inlineStr"/>
+      <c r="AKH1" t="inlineStr"/>
+      <c r="AKI1" t="inlineStr"/>
+      <c r="AKJ1" t="inlineStr"/>
+      <c r="AKK1" t="inlineStr"/>
+      <c r="AKL1" t="inlineStr"/>
+      <c r="AKM1" t="inlineStr"/>
+      <c r="AKN1" t="inlineStr"/>
+      <c r="AKO1" t="inlineStr"/>
+      <c r="AKP1" t="inlineStr"/>
+      <c r="AKQ1" t="inlineStr"/>
+      <c r="AKR1" t="inlineStr"/>
+      <c r="AKS1" t="inlineStr"/>
+      <c r="AKT1" t="inlineStr"/>
+      <c r="AKU1" t="inlineStr"/>
+      <c r="AKV1" t="inlineStr"/>
+      <c r="AKW1" t="inlineStr"/>
+      <c r="AKX1" t="inlineStr"/>
+      <c r="AKY1" t="inlineStr"/>
+      <c r="AKZ1" t="inlineStr"/>
+      <c r="ALA1" t="inlineStr"/>
+      <c r="ALB1" t="inlineStr"/>
+      <c r="ALC1" t="inlineStr"/>
+      <c r="ALD1" t="inlineStr"/>
+      <c r="ALE1" t="inlineStr"/>
+      <c r="ALF1" t="inlineStr"/>
+      <c r="ALG1" t="inlineStr"/>
+      <c r="ALH1" t="inlineStr"/>
+      <c r="ALI1" t="inlineStr"/>
+      <c r="ALJ1" t="inlineStr"/>
+      <c r="ALK1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inizio modifiche per acquisire segnali da 2 macchine
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -427,827 +427,175 @@
       <selection activeCell="LD1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="9.140625" customWidth="1" style="1" min="1" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>PMC_SPINDLE_LOAD</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>PMC_ACT_POW_X1</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>PMC_ACT_POW_Z1</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>PMC_ACT_POW_X2</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>PMC_ACT_POW_Z2</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>PMC_SPINDLE_ACT_POW</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>PMC_CUM_ACT_POW_AXES</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>PMC_CUM_POW_AXES</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>PMC_CUM_ACT_POW_X1</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>PMC_CUM_ACT_POW_Z1</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>PMC_CUM_ACT_POW_X2</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>PMC_CUM_ACT_POW_Z2</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>PMC_CUM_POW_X1</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>PMC_CUM_POW_Z1</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>PMC_CUM_POW_X2</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>PMC_CUM_POW_Z2</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>PMC_CUM_SPINDLE_ACT_POW</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>PMC_PULSECODE_TEMP_X1</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>PMC_PULSECODE_TEMP_Z1</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>PMC_PULSECODE_TEMP_X2</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>PMC_PULSECODE_TEMP_Z2</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>PMC_SERVO_TEMP_X1</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>PMC_SERVO_TEMP_Z1</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>PMC_SERVO_TEMP_X2</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>PMC_SERVO_TEMP_Z2</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>PMC_SPINDLE_MOT_TEMP</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>PMC_CURRENT_X1</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>PMC_CURRENT_Z1</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>PMC_CURRENT_E1</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>PMC_CURRENT_X2</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>PMC_CURRENT_Z2</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>PMC_CURRENT_E2</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>PMC_OVC_LEVEL</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>PMC_ACT_POW_ALL</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>CN1_1_X_WEAR</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>CN1_1_X_GEO</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>CN1_1_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>CN1_1_Z_GEO</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>CN1_2_X_WEAR</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>CN1_2_X_GEO</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>CN1_2_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>CN1_2_Z_GEO</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>CN1_3_X_WEAR</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>CN1_3_X_GEO</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>CN1_3_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>CN1_3_Z_GEO</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>CN1_4_X_WEAR</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>CN1_4_X_GEO</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>CN1_4_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>CN1_4_Z_GEO</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>CN1_5_X_WEAR</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>CN1_5_X_GEO</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>CN1_5_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>CN1_5_Z_GEO</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>CN1_6_X_WEAR</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>CN1_6_X_GEO</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>CN1_6_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>CN1_6_Z_GEO</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>CN1_7_X_WEAR</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>CN1_7_X_GEO</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>CN1_7_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>CN1_7_Z_GEO</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>CN1_8_X_WEAR</t>
-        </is>
-      </c>
-      <c r="BL1" t="inlineStr">
-        <is>
-          <t>CN1_8_X_GEO</t>
-        </is>
-      </c>
-      <c r="BM1" t="inlineStr">
-        <is>
-          <t>CN1_8_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="BN1" t="inlineStr">
-        <is>
-          <t>CN1_8_Z_GEO</t>
-        </is>
-      </c>
-      <c r="BO1" t="inlineStr">
-        <is>
-          <t>CN2_1_X_WEAR</t>
-        </is>
-      </c>
-      <c r="BP1" t="inlineStr">
-        <is>
-          <t>CN2_1_X_GEO</t>
-        </is>
-      </c>
-      <c r="BQ1" t="inlineStr">
-        <is>
-          <t>CN2_1_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="BR1" t="inlineStr">
-        <is>
-          <t>CN2_1_Z_GEO</t>
-        </is>
-      </c>
-      <c r="BS1" t="inlineStr">
-        <is>
-          <t>CN2_2_X_WEAR</t>
-        </is>
-      </c>
-      <c r="BT1" t="inlineStr">
-        <is>
-          <t>CN2_2_X_GEO</t>
-        </is>
-      </c>
-      <c r="BU1" t="inlineStr">
-        <is>
-          <t>CN2_2_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="BV1" t="inlineStr">
-        <is>
-          <t>CN2_2_Z_GEO</t>
-        </is>
-      </c>
-      <c r="BW1" t="inlineStr">
-        <is>
-          <t>CN2_3_X_WEAR</t>
-        </is>
-      </c>
-      <c r="BX1" t="inlineStr">
-        <is>
-          <t>CN2_3_X_GEO</t>
-        </is>
-      </c>
-      <c r="BY1" t="inlineStr">
-        <is>
-          <t>CN2_3_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="BZ1" t="inlineStr">
-        <is>
-          <t>CN2_3_Z_GEO</t>
-        </is>
-      </c>
-      <c r="CA1" t="inlineStr">
-        <is>
-          <t>CN2_4_X_WEAR</t>
-        </is>
-      </c>
-      <c r="CB1" t="inlineStr">
-        <is>
-          <t>CN2_4_X_GEO</t>
-        </is>
-      </c>
-      <c r="CC1" t="inlineStr">
-        <is>
-          <t>CN2_4_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="CD1" t="inlineStr">
-        <is>
-          <t>CN2_4_Z_GEO</t>
-        </is>
-      </c>
-      <c r="CE1" t="inlineStr">
-        <is>
-          <t>CN2_5_X_WEAR</t>
-        </is>
-      </c>
-      <c r="CF1" t="inlineStr">
-        <is>
-          <t>CN2_5_X_GEO</t>
-        </is>
-      </c>
-      <c r="CG1" t="inlineStr">
-        <is>
-          <t>CN2_5_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="CH1" t="inlineStr">
-        <is>
-          <t>CN2_5_Z_GEO</t>
-        </is>
-      </c>
-      <c r="CI1" t="inlineStr">
-        <is>
-          <t>CN2_6_X_WEAR</t>
-        </is>
-      </c>
-      <c r="CJ1" t="inlineStr">
-        <is>
-          <t>CN2_6_X_GEO</t>
-        </is>
-      </c>
-      <c r="CK1" t="inlineStr">
-        <is>
-          <t>CN2_6_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="CL1" t="inlineStr">
-        <is>
-          <t>CN2_6_Z_GEO</t>
-        </is>
-      </c>
-      <c r="CM1" t="inlineStr">
-        <is>
-          <t>CN2_7_X_WEAR</t>
-        </is>
-      </c>
-      <c r="CN1" t="inlineStr">
-        <is>
-          <t>CN2_7_X_GEO</t>
-        </is>
-      </c>
-      <c r="CO1" t="inlineStr">
-        <is>
-          <t>CN2_7_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="CP1" t="inlineStr">
-        <is>
-          <t>CN2_7_Z_GEO</t>
-        </is>
-      </c>
-      <c r="CQ1" t="inlineStr">
-        <is>
-          <t>CN2_8_X_WEAR</t>
-        </is>
-      </c>
-      <c r="CR1" t="inlineStr">
-        <is>
-          <t>CN2_8_X_GEO</t>
-        </is>
-      </c>
-      <c r="CS1" t="inlineStr">
-        <is>
-          <t>CN2_8_Z_WEAR</t>
-        </is>
-      </c>
-      <c r="CT1" t="inlineStr">
-        <is>
-          <t>CN2_8_Z_GEO</t>
-        </is>
-      </c>
-      <c r="CU1" t="inlineStr">
-        <is>
-          <t>PMC_RAPID_X1</t>
-        </is>
-      </c>
-      <c r="CV1" t="inlineStr">
-        <is>
-          <t>PMC_RAPID_Z1</t>
-        </is>
-      </c>
-      <c r="CW1" t="inlineStr">
-        <is>
-          <t>PMC_RAPID_X2</t>
-        </is>
-      </c>
-      <c r="CX1" t="inlineStr">
-        <is>
-          <t>PMC_RAPID_Z2</t>
-        </is>
-      </c>
-      <c r="CY1" t="inlineStr">
-        <is>
-          <t>PMC_VEL_I_GAIN_X1</t>
-        </is>
-      </c>
-      <c r="CZ1" t="inlineStr">
-        <is>
-          <t>PMC_VEL_I_GAIN_Z1</t>
-        </is>
-      </c>
-      <c r="DA1" t="inlineStr">
-        <is>
-          <t>PMC_VEL_I_GAIN_X2</t>
-        </is>
-      </c>
-      <c r="DB1" t="inlineStr">
-        <is>
-          <t>PMC_VEL_I_GAIN_Z2</t>
-        </is>
-      </c>
-      <c r="DC1" t="inlineStr">
-        <is>
-          <t>PMC_VEL_P_GAIN_X1</t>
-        </is>
-      </c>
-      <c r="DD1" t="inlineStr">
-        <is>
-          <t>PMC_VEL_P_GAIN_Z1</t>
-        </is>
-      </c>
-      <c r="DE1" t="inlineStr">
-        <is>
-          <t>PMC_VEL_P_GAIN_X2</t>
-        </is>
-      </c>
-      <c r="DF1" t="inlineStr">
-        <is>
-          <t>PMC_VEL_P_GAIN_Z2</t>
-        </is>
-      </c>
-      <c r="DG1" t="inlineStr">
-        <is>
-          <t>PMC_T1_ACC_X1</t>
-        </is>
-      </c>
-      <c r="DH1" t="inlineStr">
-        <is>
-          <t>PMC_T1_ACC_Z1</t>
-        </is>
-      </c>
-      <c r="DI1" t="inlineStr">
-        <is>
-          <t>PMC_T1_ACC_X2</t>
-        </is>
-      </c>
-      <c r="DJ1" t="inlineStr">
-        <is>
-          <t>PMC_T1_ACC_Z2</t>
-        </is>
-      </c>
-      <c r="DK1" t="inlineStr">
-        <is>
-          <t>PMC_T2_ACC_X1</t>
-        </is>
-      </c>
-      <c r="DL1" t="inlineStr">
-        <is>
-          <t>PMC_T2_ACC_Z1</t>
-        </is>
-      </c>
-      <c r="DM1" t="inlineStr">
-        <is>
-          <t>PMC_T2_ACC_X2</t>
-        </is>
-      </c>
-      <c r="DN1" t="inlineStr">
-        <is>
-          <t>PMC_T2_ACC_Z2</t>
-        </is>
-      </c>
-      <c r="DO1" t="inlineStr">
-        <is>
-          <t>PMC_MOT_LOAD_X1</t>
-        </is>
-      </c>
-      <c r="DP1" t="inlineStr">
-        <is>
-          <t>PMC_MOT_LOAD_Z1</t>
-        </is>
-      </c>
-      <c r="DQ1" t="inlineStr">
-        <is>
-          <t>PMC_MOT_LOAD_E1</t>
-        </is>
-      </c>
-      <c r="DR1" t="inlineStr">
-        <is>
-          <t>PMC_MOT_LOAD_X2</t>
-        </is>
-      </c>
-      <c r="DS1" t="inlineStr">
-        <is>
-          <t>PMC_MOT_LOAD_Z2</t>
-        </is>
-      </c>
-      <c r="DT1" t="inlineStr">
-        <is>
-          <t>PMC_MOT_LOAD_E2</t>
-        </is>
-      </c>
-      <c r="DU1" t="inlineStr">
-        <is>
-          <t>CN1_ACT_PRG_NUM</t>
-        </is>
-      </c>
-      <c r="DV1" t="inlineStr">
-        <is>
-          <t>CN2_ACT_PRG_NUM</t>
-        </is>
-      </c>
-      <c r="DW1" t="inlineStr">
-        <is>
-          <t>PMC_SVASPD[1]</t>
-        </is>
-      </c>
-      <c r="DX1" t="inlineStr">
-        <is>
-          <t>PMC_SVASPD[2]</t>
-        </is>
-      </c>
-      <c r="DY1" t="inlineStr">
-        <is>
-          <t>PMC_SVTCMD[1]</t>
-        </is>
-      </c>
-      <c r="DZ1" t="inlineStr">
-        <is>
-          <t>PMC_SVTCMD[2]</t>
-        </is>
-      </c>
-      <c r="EA1" t="inlineStr">
-        <is>
-          <t>PMC_SVOVCLV[1]</t>
-        </is>
-      </c>
-      <c r="EB1" t="inlineStr">
-        <is>
-          <t>PMC_SVOVCLV[2]</t>
-        </is>
-      </c>
-      <c r="EC1" t="inlineStr">
-        <is>
-          <t>PMC_SVTEMP[1]</t>
-        </is>
-      </c>
-      <c r="ED1" t="inlineStr">
-        <is>
-          <t>PMC_SVTEMP[2]</t>
-        </is>
-      </c>
-      <c r="EE1" t="inlineStr">
-        <is>
-          <t>PMC_SVNETPW[1]</t>
-        </is>
-      </c>
-      <c r="EF1" t="inlineStr">
-        <is>
-          <t>PMC_SVNETPW[2]</t>
-        </is>
-      </c>
-      <c r="EG1" t="inlineStr">
-        <is>
-          <t>PMC_SPASPD[1]</t>
-        </is>
-      </c>
-      <c r="EH1" t="inlineStr">
-        <is>
-          <t>PMC_SPOVCLV[1]</t>
-        </is>
-      </c>
-      <c r="EI1" t="inlineStr">
-        <is>
-          <t>PMC_SPTCMD[1]</t>
-        </is>
-      </c>
-      <c r="EJ1" t="inlineStr">
-        <is>
-          <t>PMC_SPTEMP[1]</t>
-        </is>
-      </c>
-      <c r="EK1" t="inlineStr">
-        <is>
-          <t>PMC_SPNETPW[1]</t>
-        </is>
-      </c>
-      <c r="EL1" t="inlineStr">
-        <is>
-          <t>PMC_SVASPD[3]</t>
-        </is>
-      </c>
-      <c r="EM1" t="inlineStr">
-        <is>
-          <t>PMC_SVASPD[4]</t>
-        </is>
-      </c>
-      <c r="EN1" t="inlineStr">
-        <is>
-          <t>PMC_SVTCMD[3]</t>
-        </is>
-      </c>
-      <c r="EO1" t="inlineStr">
-        <is>
-          <t>PMC_SVTCMD[4]</t>
-        </is>
-      </c>
-      <c r="EP1" t="inlineStr">
-        <is>
-          <t>PMC_SVOVCLV[3]</t>
-        </is>
-      </c>
-      <c r="EQ1" t="inlineStr">
-        <is>
-          <t>PMC_SVOVCLV[4]</t>
-        </is>
-      </c>
-      <c r="ER1" t="inlineStr">
-        <is>
-          <t>PMC_SVTEMP[3]</t>
-        </is>
-      </c>
-      <c r="ES1" t="inlineStr">
-        <is>
-          <t>PMC_SVTEMP[4]</t>
-        </is>
-      </c>
-      <c r="ET1" t="inlineStr">
-        <is>
-          <t>PMC_SVNETPW[3]</t>
-        </is>
-      </c>
-      <c r="EU1" t="inlineStr">
-        <is>
-          <t>PMC_SVNETPW[4]</t>
-        </is>
-      </c>
-      <c r="EV1" t="inlineStr">
-        <is>
-          <t>CN1_NUM_MACHINED_PARTS</t>
-        </is>
-      </c>
-      <c r="EW1" t="inlineStr">
-        <is>
-          <t>CN2_NUM_MACHINED_PARTS</t>
-        </is>
-      </c>
-      <c r="EX1" t="inlineStr">
-        <is>
-          <t>CN_MACHINING_START</t>
-        </is>
-      </c>
-      <c r="EY1" t="inlineStr">
-        <is>
-          <t>CN_MACHINING_STOP</t>
-        </is>
-      </c>
-      <c r="EZ1" t="inlineStr">
-        <is>
-          <t>RESET_DURING_CYCLE</t>
-        </is>
-      </c>
-      <c r="FA1" t="inlineStr">
-        <is>
-          <t>PMC_X1_BEAR_TEMP</t>
-        </is>
-      </c>
-      <c r="FB1" t="inlineStr">
-        <is>
-          <t>PMC_Z1_BEAR_TEMP</t>
-        </is>
-      </c>
-      <c r="FC1" t="inlineStr">
-        <is>
-          <t>PMC_X2_BEAR_TEMP</t>
-        </is>
-      </c>
-      <c r="FD1" t="inlineStr">
-        <is>
-          <t>PMC_Z2_BEAR_TEMP</t>
-        </is>
-      </c>
-      <c r="FE1" t="inlineStr">
-        <is>
-          <t>PMC_SPINDLE_TEMP</t>
-        </is>
-      </c>
-      <c r="FF1" t="inlineStr">
-        <is>
-          <t>PMC_SPINDLE_RMS_VIB</t>
-        </is>
-      </c>
-      <c r="FG1" t="inlineStr">
-        <is>
-          <t>PMC_SPINDLE_MAX_VIB</t>
-        </is>
-      </c>
+      <c r="A1" t="inlineStr"/>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr"/>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr"/>
+      <c r="F1" t="inlineStr"/>
+      <c r="G1" t="inlineStr"/>
+      <c r="H1" t="inlineStr"/>
+      <c r="I1" t="inlineStr"/>
+      <c r="J1" t="inlineStr"/>
+      <c r="K1" t="inlineStr"/>
+      <c r="L1" t="inlineStr"/>
+      <c r="M1" t="inlineStr"/>
+      <c r="N1" t="inlineStr"/>
+      <c r="O1" t="inlineStr"/>
+      <c r="P1" t="inlineStr"/>
+      <c r="Q1" t="inlineStr"/>
+      <c r="R1" t="inlineStr"/>
+      <c r="S1" t="inlineStr"/>
+      <c r="T1" t="inlineStr"/>
+      <c r="U1" t="inlineStr"/>
+      <c r="V1" t="inlineStr"/>
+      <c r="W1" t="inlineStr"/>
+      <c r="X1" t="inlineStr"/>
+      <c r="Y1" t="inlineStr"/>
+      <c r="Z1" t="inlineStr"/>
+      <c r="AA1" t="inlineStr"/>
+      <c r="AB1" t="inlineStr"/>
+      <c r="AC1" t="inlineStr"/>
+      <c r="AD1" t="inlineStr"/>
+      <c r="AE1" t="inlineStr"/>
+      <c r="AF1" t="inlineStr"/>
+      <c r="AG1" t="inlineStr"/>
+      <c r="AH1" t="inlineStr"/>
+      <c r="AI1" t="inlineStr"/>
+      <c r="AJ1" t="inlineStr"/>
+      <c r="AK1" t="inlineStr"/>
+      <c r="AL1" t="inlineStr"/>
+      <c r="AM1" t="inlineStr"/>
+      <c r="AN1" t="inlineStr"/>
+      <c r="AO1" t="inlineStr"/>
+      <c r="AP1" t="inlineStr"/>
+      <c r="AQ1" t="inlineStr"/>
+      <c r="AR1" t="inlineStr"/>
+      <c r="AS1" t="inlineStr"/>
+      <c r="AT1" t="inlineStr"/>
+      <c r="AU1" t="inlineStr"/>
+      <c r="AV1" t="inlineStr"/>
+      <c r="AW1" t="inlineStr"/>
+      <c r="AX1" t="inlineStr"/>
+      <c r="AY1" t="inlineStr"/>
+      <c r="AZ1" t="inlineStr"/>
+      <c r="BA1" t="inlineStr"/>
+      <c r="BB1" t="inlineStr"/>
+      <c r="BC1" t="inlineStr"/>
+      <c r="BD1" t="inlineStr"/>
+      <c r="BE1" t="inlineStr"/>
+      <c r="BF1" t="inlineStr"/>
+      <c r="BG1" t="inlineStr"/>
+      <c r="BH1" t="inlineStr"/>
+      <c r="BI1" t="inlineStr"/>
+      <c r="BJ1" t="inlineStr"/>
+      <c r="BK1" t="inlineStr"/>
+      <c r="BL1" t="inlineStr"/>
+      <c r="BM1" t="inlineStr"/>
+      <c r="BN1" t="inlineStr"/>
+      <c r="BO1" t="inlineStr"/>
+      <c r="BP1" t="inlineStr"/>
+      <c r="BQ1" t="inlineStr"/>
+      <c r="BR1" t="inlineStr"/>
+      <c r="BS1" t="inlineStr"/>
+      <c r="BT1" t="inlineStr"/>
+      <c r="BU1" t="inlineStr"/>
+      <c r="BV1" t="inlineStr"/>
+      <c r="BW1" t="inlineStr"/>
+      <c r="BX1" t="inlineStr"/>
+      <c r="BY1" t="inlineStr"/>
+      <c r="BZ1" t="inlineStr"/>
+      <c r="CA1" t="inlineStr"/>
+      <c r="CB1" t="inlineStr"/>
+      <c r="CC1" t="inlineStr"/>
+      <c r="CD1" t="inlineStr"/>
+      <c r="CE1" t="inlineStr"/>
+      <c r="CF1" t="inlineStr"/>
+      <c r="CG1" t="inlineStr"/>
+      <c r="CH1" t="inlineStr"/>
+      <c r="CI1" t="inlineStr"/>
+      <c r="CJ1" t="inlineStr"/>
+      <c r="CK1" t="inlineStr"/>
+      <c r="CL1" t="inlineStr"/>
+      <c r="CM1" t="inlineStr"/>
+      <c r="CN1" t="inlineStr"/>
+      <c r="CO1" t="inlineStr"/>
+      <c r="CP1" t="inlineStr"/>
+      <c r="CQ1" t="inlineStr"/>
+      <c r="CR1" t="inlineStr"/>
+      <c r="CS1" t="inlineStr"/>
+      <c r="CT1" t="inlineStr"/>
+      <c r="CU1" t="inlineStr"/>
+      <c r="CV1" t="inlineStr"/>
+      <c r="CW1" t="inlineStr"/>
+      <c r="CX1" t="inlineStr"/>
+      <c r="CY1" t="inlineStr"/>
+      <c r="CZ1" t="inlineStr"/>
+      <c r="DA1" t="inlineStr"/>
+      <c r="DB1" t="inlineStr"/>
+      <c r="DC1" t="inlineStr"/>
+      <c r="DD1" t="inlineStr"/>
+      <c r="DE1" t="inlineStr"/>
+      <c r="DF1" t="inlineStr"/>
+      <c r="DG1" t="inlineStr"/>
+      <c r="DH1" t="inlineStr"/>
+      <c r="DI1" t="inlineStr"/>
+      <c r="DJ1" t="inlineStr"/>
+      <c r="DK1" t="inlineStr"/>
+      <c r="DL1" t="inlineStr"/>
+      <c r="DM1" t="inlineStr"/>
+      <c r="DN1" t="inlineStr"/>
+      <c r="DO1" t="inlineStr"/>
+      <c r="DP1" t="inlineStr"/>
+      <c r="DQ1" t="inlineStr"/>
+      <c r="DR1" t="inlineStr"/>
+      <c r="DS1" t="inlineStr"/>
+      <c r="DT1" t="inlineStr"/>
+      <c r="DU1" t="inlineStr"/>
+      <c r="DV1" t="inlineStr"/>
+      <c r="DW1" t="inlineStr"/>
+      <c r="DX1" t="inlineStr"/>
+      <c r="DY1" t="inlineStr"/>
+      <c r="DZ1" t="inlineStr"/>
+      <c r="EA1" t="inlineStr"/>
+      <c r="EB1" t="inlineStr"/>
+      <c r="EC1" t="inlineStr"/>
+      <c r="ED1" t="inlineStr"/>
+      <c r="EE1" t="inlineStr"/>
+      <c r="EF1" t="inlineStr"/>
+      <c r="EG1" t="inlineStr"/>
+      <c r="EH1" t="inlineStr"/>
+      <c r="EI1" t="inlineStr"/>
+      <c r="EJ1" t="inlineStr"/>
+      <c r="EK1" t="inlineStr"/>
+      <c r="EL1" t="inlineStr"/>
+      <c r="EM1" t="inlineStr"/>
+      <c r="EN1" t="inlineStr"/>
+      <c r="EO1" t="inlineStr"/>
+      <c r="EP1" t="inlineStr"/>
+      <c r="EQ1" t="inlineStr"/>
+      <c r="ER1" t="inlineStr"/>
+      <c r="ES1" t="inlineStr"/>
+      <c r="ET1" t="inlineStr"/>
+      <c r="EU1" t="inlineStr"/>
+      <c r="EV1" t="inlineStr"/>
+      <c r="EW1" t="inlineStr"/>
+      <c r="EX1" t="inlineStr"/>
+      <c r="EY1" t="inlineStr"/>
+      <c r="EZ1" t="inlineStr"/>
+      <c r="FA1" t="inlineStr"/>
+      <c r="FB1" t="inlineStr"/>
+      <c r="FC1" t="inlineStr"/>
+      <c r="FD1" t="inlineStr"/>
+      <c r="FE1" t="inlineStr"/>
+      <c r="FF1" t="inlineStr"/>
+      <c r="FG1" t="inlineStr"/>
       <c r="FH1" t="inlineStr"/>
       <c r="FI1" t="inlineStr"/>
       <c r="FJ1" t="inlineStr"/>
@@ -2105,10 +1453,10 @@
         <v>2162688</v>
       </c>
       <c r="G2" t="n">
-        <v>2164922</v>
+        <v>2162733</v>
       </c>
       <c r="H2" t="n">
-        <v>2164996</v>
+        <v>2162733</v>
       </c>
       <c r="I2" t="n">
         <v>2162688</v>
@@ -2135,13 +1483,13 @@
         <v>2162688</v>
       </c>
       <c r="Q2" t="n">
-        <v>2234</v>
+        <v>45</v>
       </c>
       <c r="R2" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="S2" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="T2" t="n">
         <v>132</v>
@@ -2150,43 +1498,43 @@
         <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="W2" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="X2" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Y2" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Z2" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="AA2" t="n">
-        <v>170</v>
+        <v>1</v>
       </c>
       <c r="AB2" t="n">
-        <v>242</v>
+        <v>2</v>
       </c>
       <c r="AC2" t="n">
-        <v>64974</v>
+        <v>230</v>
       </c>
       <c r="AD2" t="n">
-        <v>65535</v>
+        <v>3</v>
       </c>
       <c r="AE2" t="n">
-        <v>201</v>
+        <v>483</v>
       </c>
       <c r="AF2" t="n">
-        <v>65243</v>
+        <v>0</v>
       </c>
       <c r="AG2" t="n">
         <v>10223616</v>
       </c>
       <c r="AH2" t="n">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="AI2" t="inlineStr">
         <is>
@@ -2588,12 +1936,12 @@
       </c>
       <c r="DU2" t="inlineStr">
         <is>
-          <t>O1103</t>
+          <t>O4084</t>
         </is>
       </c>
       <c r="DV2" t="inlineStr">
         <is>
-          <t>O2103</t>
+          <t>O5084</t>
         </is>
       </c>
       <c r="DW2" t="inlineStr">
@@ -2623,17 +1971,17 @@
       </c>
       <c r="EB2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="EC2" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>25</t>
         </is>
       </c>
       <c r="ED2" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>34</t>
         </is>
       </c>
       <c r="EE2" t="inlineStr">
@@ -2663,12 +2011,12 @@
       </c>
       <c r="EJ2" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>26</t>
         </is>
       </c>
       <c r="EK2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>250</t>
         </is>
       </c>
       <c r="EL2" t="inlineStr">
@@ -2737,25 +2085,25 @@
         <v>0</v>
       </c>
       <c r="FA2" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="FB2" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="FC2" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="FD2" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="FE2" t="n">
-        <v>2521</v>
+        <v>2539</v>
       </c>
       <c r="FF2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="FG2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
classi funzionanti sia di connessione che di manage dei file excel
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -423,13 +423,14 @@
   </sheetPr>
   <dimension ref="A1:ALK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="LD1" workbookViewId="0">
-      <selection activeCell="LD1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="9.140625" customWidth="1" style="1" min="1" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="1" max="3"/>
+    <col width="9.140625" customWidth="1" style="1" min="4" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1434,677 +1435,1005 @@
       <c r="ALK1" t="inlineStr"/>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2162688</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>67698688</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2162688</v>
-      </c>
-      <c r="F2" t="n">
-        <v>2162688</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2162733</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2162733</v>
-      </c>
-      <c r="I2" t="n">
-        <v>2162688</v>
-      </c>
-      <c r="J2" t="n">
-        <v>67698688</v>
-      </c>
-      <c r="K2" t="n">
-        <v>67698688</v>
-      </c>
-      <c r="L2" t="n">
-        <v>2162688</v>
-      </c>
-      <c r="M2" t="n">
-        <v>2162688</v>
-      </c>
-      <c r="N2" t="n">
-        <v>67698688</v>
-      </c>
-      <c r="O2" t="n">
-        <v>67698688</v>
-      </c>
-      <c r="P2" t="n">
-        <v>2162688</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>45</v>
-      </c>
-      <c r="R2" t="n">
-        <v>25</v>
-      </c>
-      <c r="S2" t="n">
-        <v>34</v>
-      </c>
-      <c r="T2" t="n">
-        <v>132</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="n">
-        <v>31</v>
-      </c>
-      <c r="W2" t="n">
-        <v>40</v>
-      </c>
-      <c r="X2" t="n">
-        <v>32</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>39</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>26</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>230</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>483</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>10223616</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>208.750</t>
-        </is>
-      </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AL2" t="inlineStr">
-        <is>
-          <t>132.180</t>
-        </is>
-      </c>
-      <c r="AM2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AN2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AO2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AP2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AQ2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AR2" t="inlineStr">
-        <is>
-          <t>-9.910</t>
-        </is>
-      </c>
-      <c r="AS2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AT2" t="inlineStr">
-        <is>
-          <t>295.980</t>
-        </is>
-      </c>
-      <c r="AU2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AV2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AW2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AX2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AY2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="AZ2" t="inlineStr">
-        <is>
-          <t>211.440</t>
-        </is>
-      </c>
-      <c r="BA2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BB2" t="inlineStr">
-        <is>
-          <t>147.110</t>
-        </is>
-      </c>
-      <c r="BC2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BD2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BE2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BF2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BG2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BH2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BI2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BJ2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BK2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BL2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BM2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BN2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BO2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BP2" t="inlineStr">
-        <is>
-          <t>16.010</t>
-        </is>
-      </c>
-      <c r="BQ2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BR2" t="inlineStr">
-        <is>
-          <t>301.430</t>
-        </is>
-      </c>
-      <c r="BS2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BT2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BU2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BV2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BW2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BX2" t="inlineStr">
-        <is>
-          <t>12.190</t>
-        </is>
-      </c>
-      <c r="BY2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="BZ2" t="inlineStr">
-        <is>
-          <t>289.490</t>
-        </is>
-      </c>
-      <c r="CA2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CB2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CC2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CD2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CE2" t="inlineStr">
-        <is>
-          <t>0.100</t>
-        </is>
-      </c>
-      <c r="CF2" t="inlineStr">
-        <is>
-          <t>4.340</t>
-        </is>
-      </c>
-      <c r="CG2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CH2" t="inlineStr">
-        <is>
-          <t>274.060</t>
-        </is>
-      </c>
-      <c r="CI2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CJ2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CK2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CL2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CM2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CN2" t="inlineStr">
-        <is>
-          <t>-45.000</t>
-        </is>
-      </c>
-      <c r="CO2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CP2" t="inlineStr">
-        <is>
-          <t>268.100</t>
-        </is>
-      </c>
-      <c r="CQ2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CR2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CS2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CT2" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="CU2" t="n">
-        <v>30000000</v>
-      </c>
-      <c r="CV2" t="n">
-        <v>196610</v>
-      </c>
-      <c r="CW2" t="n">
-        <v>1420</v>
-      </c>
-      <c r="CX2" t="n">
-        <v>393216</v>
-      </c>
-      <c r="CY2" t="n">
-        <v>193</v>
-      </c>
-      <c r="CZ2" t="n">
-        <v>197</v>
-      </c>
-      <c r="DA2" t="n">
-        <v>193</v>
-      </c>
-      <c r="DB2" t="n">
-        <v>197</v>
-      </c>
-      <c r="DC2" t="n">
-        <v>63809</v>
-      </c>
-      <c r="DD2" t="n">
-        <v>63771</v>
-      </c>
-      <c r="DE2" t="n">
-        <v>63809</v>
-      </c>
-      <c r="DF2" t="n">
-        <v>63771</v>
-      </c>
-      <c r="DG2" t="n">
-        <v>350</v>
-      </c>
-      <c r="DH2" t="n">
-        <v>350</v>
-      </c>
-      <c r="DI2" t="n">
-        <v>350</v>
-      </c>
-      <c r="DJ2" t="n">
-        <v>350</v>
-      </c>
-      <c r="DK2" t="n">
-        <v>300</v>
-      </c>
-      <c r="DL2" t="n">
-        <v>300</v>
-      </c>
-      <c r="DM2" t="n">
-        <v>300</v>
-      </c>
-      <c r="DN2" t="n">
-        <v>300</v>
-      </c>
-      <c r="DO2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DP2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DQ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DR2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DS2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DT2" t="n">
-        <v>0</v>
-      </c>
-      <c r="DU2" t="inlineStr">
-        <is>
-          <t>O4084</t>
-        </is>
-      </c>
-      <c r="DV2" t="inlineStr">
-        <is>
-          <t>O5084</t>
-        </is>
-      </c>
-      <c r="DW2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="DX2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="DY2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="DZ2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EA2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EB2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="EC2" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="ED2" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="EE2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EF2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EG2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EH2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EI2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EJ2" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="EK2" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
-      </c>
-      <c r="EL2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EM2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EN2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EO2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EP2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EQ2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="ER2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="ES2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="ET2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EU2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="EV2" t="n">
-        <v>22</v>
-      </c>
-      <c r="EW2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX2" t="b">
-        <v>0</v>
-      </c>
-      <c r="EY2" t="b">
-        <v>0</v>
-      </c>
-      <c r="EZ2" t="b">
-        <v>0</v>
-      </c>
-      <c r="FA2" t="n">
-        <v>27</v>
-      </c>
-      <c r="FB2" t="n">
-        <v>29</v>
-      </c>
-      <c r="FC2" t="n">
-        <v>27</v>
-      </c>
-      <c r="FD2" t="n">
-        <v>29</v>
-      </c>
-      <c r="FE2" t="n">
-        <v>2539</v>
-      </c>
-      <c r="FF2" t="n">
-        <v>6</v>
-      </c>
-      <c r="FG2" t="n">
-        <v>17</v>
-      </c>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr"/>
+      <c r="BA2" t="inlineStr"/>
+      <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr"/>
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr"/>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr"/>
+      <c r="BH2" t="inlineStr"/>
+      <c r="BI2" t="inlineStr"/>
+      <c r="BJ2" t="inlineStr"/>
+      <c r="BK2" t="inlineStr"/>
+      <c r="BL2" t="inlineStr"/>
+      <c r="BM2" t="inlineStr"/>
+      <c r="BN2" t="inlineStr"/>
+      <c r="BO2" t="inlineStr"/>
+      <c r="BP2" t="inlineStr"/>
+      <c r="BQ2" t="inlineStr"/>
+      <c r="BR2" t="inlineStr"/>
+      <c r="BS2" t="inlineStr"/>
+      <c r="BT2" t="inlineStr"/>
+      <c r="BU2" t="inlineStr"/>
+      <c r="BV2" t="inlineStr"/>
+      <c r="BW2" t="inlineStr"/>
+      <c r="BX2" t="inlineStr"/>
+      <c r="BY2" t="inlineStr"/>
+      <c r="BZ2" t="inlineStr"/>
+      <c r="CA2" t="inlineStr"/>
+      <c r="CB2" t="inlineStr"/>
+      <c r="CC2" t="inlineStr"/>
+      <c r="CD2" t="inlineStr"/>
+      <c r="CE2" t="inlineStr"/>
+      <c r="CF2" t="inlineStr"/>
+      <c r="CG2" t="inlineStr"/>
+      <c r="CH2" t="inlineStr"/>
+      <c r="CI2" t="inlineStr"/>
+      <c r="CJ2" t="inlineStr"/>
+      <c r="CK2" t="inlineStr"/>
+      <c r="CL2" t="inlineStr"/>
+      <c r="CM2" t="inlineStr"/>
+      <c r="CN2" t="inlineStr"/>
+      <c r="CO2" t="inlineStr"/>
+      <c r="CP2" t="inlineStr"/>
+      <c r="CQ2" t="inlineStr"/>
+      <c r="CR2" t="inlineStr"/>
+      <c r="CS2" t="inlineStr"/>
+      <c r="CT2" t="inlineStr"/>
+      <c r="CU2" t="inlineStr"/>
+      <c r="CV2" t="inlineStr"/>
+      <c r="CW2" t="inlineStr"/>
+      <c r="CX2" t="inlineStr"/>
+      <c r="CY2" t="inlineStr"/>
+      <c r="CZ2" t="inlineStr"/>
+      <c r="DA2" t="inlineStr"/>
+      <c r="DB2" t="inlineStr"/>
+      <c r="DC2" t="inlineStr"/>
+      <c r="DD2" t="inlineStr"/>
+      <c r="DE2" t="inlineStr"/>
+      <c r="DF2" t="inlineStr"/>
+      <c r="DG2" t="inlineStr"/>
+      <c r="DH2" t="inlineStr"/>
+      <c r="DI2" t="inlineStr"/>
+      <c r="DJ2" t="inlineStr"/>
+      <c r="DK2" t="inlineStr"/>
+      <c r="DL2" t="inlineStr"/>
+      <c r="DM2" t="inlineStr"/>
+      <c r="DN2" t="inlineStr"/>
+      <c r="DO2" t="inlineStr"/>
+      <c r="DP2" t="inlineStr"/>
+      <c r="DQ2" t="inlineStr"/>
+      <c r="DR2" t="inlineStr"/>
+      <c r="DS2" t="inlineStr"/>
+      <c r="DT2" t="inlineStr"/>
+      <c r="DU2" t="inlineStr"/>
+      <c r="DV2" t="inlineStr"/>
+      <c r="DW2" t="inlineStr"/>
+      <c r="DX2" t="inlineStr"/>
+      <c r="DY2" t="inlineStr"/>
+      <c r="DZ2" t="inlineStr"/>
+      <c r="EA2" t="inlineStr"/>
+      <c r="EB2" t="inlineStr"/>
+      <c r="EC2" t="inlineStr"/>
+      <c r="ED2" t="inlineStr"/>
+      <c r="EE2" t="inlineStr"/>
+      <c r="EF2" t="inlineStr"/>
+      <c r="EG2" t="inlineStr"/>
+      <c r="EH2" t="inlineStr"/>
+      <c r="EI2" t="inlineStr"/>
+      <c r="EJ2" t="inlineStr"/>
+      <c r="EK2" t="inlineStr"/>
+      <c r="EL2" t="inlineStr"/>
+      <c r="EM2" t="inlineStr"/>
+      <c r="EN2" t="inlineStr"/>
+      <c r="EO2" t="inlineStr"/>
+      <c r="EP2" t="inlineStr"/>
+      <c r="EQ2" t="inlineStr"/>
+      <c r="ER2" t="inlineStr"/>
+      <c r="ES2" t="inlineStr"/>
+      <c r="ET2" t="inlineStr"/>
+      <c r="EU2" t="inlineStr"/>
+      <c r="EV2" t="inlineStr"/>
+      <c r="EW2" t="inlineStr"/>
+      <c r="EX2" t="inlineStr"/>
+      <c r="EY2" t="inlineStr"/>
+      <c r="EZ2" t="inlineStr"/>
+      <c r="FA2" t="inlineStr"/>
+      <c r="FB2" t="inlineStr"/>
+      <c r="FC2" t="inlineStr"/>
+      <c r="FD2" t="inlineStr"/>
+      <c r="FE2" t="inlineStr"/>
+      <c r="FF2" t="inlineStr"/>
+      <c r="FG2" t="inlineStr"/>
+      <c r="FH2" t="inlineStr"/>
+      <c r="FI2" t="inlineStr"/>
+      <c r="FJ2" t="inlineStr"/>
+      <c r="FK2" t="inlineStr"/>
+      <c r="FL2" t="inlineStr"/>
+      <c r="FM2" t="inlineStr"/>
+      <c r="FN2" t="inlineStr"/>
+      <c r="FO2" t="inlineStr"/>
+      <c r="FP2" t="inlineStr"/>
+      <c r="FQ2" t="inlineStr"/>
+      <c r="FR2" t="inlineStr"/>
+      <c r="FS2" t="inlineStr"/>
+      <c r="FT2" t="inlineStr"/>
+      <c r="FU2" t="inlineStr"/>
+      <c r="FV2" t="inlineStr"/>
+      <c r="FW2" t="inlineStr"/>
+      <c r="FX2" t="inlineStr"/>
+      <c r="FY2" t="inlineStr"/>
+      <c r="FZ2" t="inlineStr"/>
+      <c r="GA2" t="inlineStr"/>
+      <c r="GB2" t="inlineStr"/>
+      <c r="GC2" t="inlineStr"/>
+      <c r="GD2" t="inlineStr"/>
+      <c r="GE2" t="inlineStr"/>
+      <c r="GF2" t="inlineStr"/>
+      <c r="GG2" t="inlineStr"/>
+      <c r="GH2" t="inlineStr"/>
+      <c r="GI2" t="inlineStr"/>
+      <c r="GJ2" t="inlineStr"/>
+      <c r="GK2" t="inlineStr"/>
+      <c r="GL2" t="inlineStr"/>
+      <c r="GM2" t="inlineStr"/>
+      <c r="GN2" t="inlineStr"/>
+      <c r="GO2" t="inlineStr"/>
+      <c r="GP2" t="inlineStr"/>
+      <c r="GQ2" t="inlineStr"/>
+      <c r="GR2" t="inlineStr"/>
+      <c r="GS2" t="inlineStr"/>
+      <c r="GT2" t="inlineStr"/>
+      <c r="GU2" t="inlineStr"/>
+      <c r="GV2" t="inlineStr"/>
+      <c r="GW2" t="inlineStr"/>
+      <c r="GX2" t="inlineStr"/>
+      <c r="GY2" t="inlineStr"/>
+      <c r="GZ2" t="inlineStr"/>
+      <c r="HA2" t="inlineStr"/>
+      <c r="HB2" t="inlineStr"/>
+      <c r="HC2" t="inlineStr"/>
+      <c r="HD2" t="inlineStr"/>
+      <c r="HE2" t="inlineStr"/>
+      <c r="HF2" t="inlineStr"/>
+      <c r="HG2" t="inlineStr"/>
+      <c r="HH2" t="inlineStr"/>
+      <c r="HI2" t="inlineStr"/>
+      <c r="HJ2" t="inlineStr"/>
+      <c r="HK2" t="inlineStr"/>
+      <c r="HL2" t="inlineStr"/>
+      <c r="HM2" t="inlineStr"/>
+      <c r="HN2" t="inlineStr"/>
+      <c r="HO2" t="inlineStr"/>
+      <c r="HP2" t="inlineStr"/>
+      <c r="HQ2" t="inlineStr"/>
+      <c r="HR2" t="inlineStr"/>
+      <c r="HS2" t="inlineStr"/>
+      <c r="HT2" t="inlineStr"/>
+      <c r="HU2" t="inlineStr"/>
+      <c r="HV2" t="inlineStr"/>
+      <c r="HW2" t="inlineStr"/>
+      <c r="HX2" t="inlineStr"/>
+      <c r="HY2" t="inlineStr"/>
+      <c r="HZ2" t="inlineStr"/>
+      <c r="IA2" t="inlineStr"/>
+      <c r="IB2" t="inlineStr"/>
+      <c r="IC2" t="inlineStr"/>
+      <c r="ID2" t="inlineStr"/>
+      <c r="IE2" t="inlineStr"/>
+      <c r="IF2" t="inlineStr"/>
+      <c r="IG2" t="inlineStr"/>
+      <c r="IH2" t="inlineStr"/>
+      <c r="II2" t="inlineStr"/>
+      <c r="IJ2" t="inlineStr"/>
+      <c r="IK2" t="inlineStr"/>
+      <c r="IL2" t="inlineStr"/>
+      <c r="IM2" t="inlineStr"/>
+      <c r="IN2" t="inlineStr"/>
+      <c r="IO2" t="inlineStr"/>
+      <c r="IP2" t="inlineStr"/>
+      <c r="IQ2" t="inlineStr"/>
+      <c r="IR2" t="inlineStr"/>
+      <c r="IS2" t="inlineStr"/>
+      <c r="IT2" t="inlineStr"/>
+      <c r="IU2" t="inlineStr"/>
+      <c r="IV2" t="inlineStr"/>
+      <c r="IW2" t="inlineStr"/>
+      <c r="IX2" t="inlineStr"/>
+      <c r="IY2" t="inlineStr"/>
+      <c r="IZ2" t="inlineStr"/>
+      <c r="JA2" t="inlineStr"/>
+      <c r="JB2" t="inlineStr"/>
+      <c r="JC2" t="inlineStr"/>
+      <c r="JD2" t="inlineStr"/>
+      <c r="JE2" t="inlineStr"/>
+      <c r="JF2" t="inlineStr"/>
+      <c r="JG2" t="inlineStr"/>
+      <c r="JH2" t="inlineStr"/>
+      <c r="JI2" t="inlineStr"/>
+      <c r="JJ2" t="inlineStr"/>
+      <c r="JK2" t="inlineStr"/>
+      <c r="JL2" t="inlineStr"/>
+      <c r="JM2" t="inlineStr"/>
+      <c r="JN2" t="inlineStr"/>
+      <c r="JO2" t="inlineStr"/>
+      <c r="JP2" t="inlineStr"/>
+      <c r="JQ2" t="inlineStr"/>
+      <c r="JR2" t="inlineStr"/>
+      <c r="JS2" t="inlineStr"/>
+      <c r="JT2" t="inlineStr"/>
+      <c r="JU2" t="inlineStr"/>
+      <c r="JV2" t="inlineStr"/>
+      <c r="JW2" t="inlineStr"/>
+      <c r="JX2" t="inlineStr"/>
+      <c r="JY2" t="inlineStr"/>
+      <c r="JZ2" t="inlineStr"/>
+      <c r="KA2" t="inlineStr"/>
+      <c r="KB2" t="inlineStr"/>
+      <c r="KC2" t="inlineStr"/>
+      <c r="KD2" t="inlineStr"/>
+      <c r="KE2" t="inlineStr"/>
+      <c r="KF2" t="inlineStr"/>
+      <c r="KG2" t="inlineStr"/>
+      <c r="KH2" t="inlineStr"/>
+      <c r="KI2" t="inlineStr"/>
+      <c r="KJ2" t="inlineStr"/>
+      <c r="KK2" t="inlineStr"/>
+      <c r="KL2" t="inlineStr"/>
+      <c r="KM2" t="inlineStr"/>
+      <c r="KN2" t="inlineStr"/>
+      <c r="KO2" t="inlineStr"/>
+      <c r="KP2" t="inlineStr"/>
+      <c r="KQ2" t="inlineStr"/>
+      <c r="KR2" t="inlineStr"/>
+      <c r="KS2" t="inlineStr"/>
+      <c r="KT2" t="inlineStr"/>
+      <c r="KU2" t="inlineStr"/>
+      <c r="KV2" t="inlineStr"/>
+      <c r="KW2" t="inlineStr"/>
+      <c r="KX2" t="inlineStr"/>
+      <c r="KY2" t="inlineStr"/>
+      <c r="KZ2" t="inlineStr"/>
+      <c r="LA2" t="inlineStr"/>
+      <c r="LB2" t="inlineStr"/>
+      <c r="LC2" t="inlineStr"/>
+      <c r="LD2" t="inlineStr"/>
+      <c r="LE2" t="inlineStr"/>
+      <c r="LF2" t="inlineStr"/>
+      <c r="LG2" t="inlineStr"/>
+      <c r="LH2" t="inlineStr"/>
+      <c r="LI2" t="inlineStr"/>
+      <c r="LJ2" t="inlineStr"/>
+      <c r="LK2" t="inlineStr"/>
+      <c r="LL2" t="inlineStr"/>
+      <c r="LM2" t="inlineStr"/>
+      <c r="LN2" t="inlineStr"/>
+      <c r="LO2" t="inlineStr"/>
+      <c r="LP2" t="inlineStr"/>
+      <c r="LQ2" t="inlineStr"/>
+      <c r="LR2" t="inlineStr"/>
+      <c r="LS2" t="inlineStr"/>
+      <c r="LT2" t="inlineStr"/>
+      <c r="LU2" t="inlineStr"/>
+      <c r="LV2" t="inlineStr"/>
+      <c r="LW2" t="inlineStr"/>
+      <c r="LX2" t="inlineStr"/>
+      <c r="LY2" t="inlineStr"/>
+      <c r="LZ2" t="inlineStr"/>
+      <c r="MA2" t="inlineStr"/>
+      <c r="MB2" t="inlineStr"/>
+      <c r="MC2" t="inlineStr"/>
+      <c r="MD2" t="inlineStr"/>
+      <c r="ME2" t="inlineStr"/>
+      <c r="MF2" t="inlineStr"/>
+      <c r="MG2" t="inlineStr"/>
+      <c r="MH2" t="inlineStr"/>
+      <c r="MI2" t="inlineStr"/>
+      <c r="MJ2" t="inlineStr"/>
+      <c r="MK2" t="inlineStr"/>
+      <c r="ML2" t="inlineStr"/>
+      <c r="MM2" t="inlineStr"/>
+      <c r="MN2" t="inlineStr"/>
+      <c r="MO2" t="inlineStr"/>
+      <c r="MP2" t="inlineStr"/>
+      <c r="MQ2" t="inlineStr"/>
+      <c r="MR2" t="inlineStr"/>
+      <c r="MS2" t="inlineStr"/>
+      <c r="MT2" t="inlineStr"/>
+      <c r="MU2" t="inlineStr"/>
+      <c r="MV2" t="inlineStr"/>
+      <c r="MW2" t="inlineStr"/>
+      <c r="MX2" t="inlineStr"/>
+      <c r="MY2" t="inlineStr"/>
+      <c r="MZ2" t="inlineStr"/>
+      <c r="NA2" t="inlineStr"/>
+      <c r="NB2" t="inlineStr"/>
+      <c r="NC2" t="inlineStr"/>
+      <c r="ND2" t="inlineStr"/>
+      <c r="NE2" t="inlineStr"/>
+      <c r="NF2" t="inlineStr"/>
+      <c r="NG2" t="inlineStr"/>
+      <c r="NH2" t="inlineStr"/>
+      <c r="NI2" t="inlineStr"/>
+      <c r="NJ2" t="inlineStr"/>
+      <c r="NK2" t="inlineStr"/>
+      <c r="NL2" t="inlineStr"/>
+      <c r="NM2" t="inlineStr"/>
+      <c r="NN2" t="inlineStr"/>
+      <c r="NO2" t="inlineStr"/>
+      <c r="NP2" t="inlineStr"/>
+      <c r="NQ2" t="inlineStr"/>
+      <c r="NR2" t="inlineStr"/>
+      <c r="NS2" t="inlineStr"/>
+      <c r="NT2" t="inlineStr"/>
+      <c r="NU2" t="inlineStr"/>
+      <c r="NV2" t="inlineStr"/>
+      <c r="NW2" t="inlineStr"/>
+      <c r="NX2" t="inlineStr"/>
+      <c r="NY2" t="inlineStr"/>
+      <c r="NZ2" t="inlineStr"/>
+      <c r="OA2" t="inlineStr"/>
+      <c r="OB2" t="inlineStr"/>
+      <c r="OC2" t="inlineStr"/>
+      <c r="OD2" t="inlineStr"/>
+      <c r="OE2" t="inlineStr"/>
+      <c r="OF2" t="inlineStr"/>
+      <c r="OG2" t="inlineStr"/>
+      <c r="OH2" t="inlineStr"/>
+      <c r="OI2" t="inlineStr"/>
+      <c r="OJ2" t="inlineStr"/>
+      <c r="OK2" t="inlineStr"/>
+      <c r="OL2" t="inlineStr"/>
+      <c r="OM2" t="inlineStr"/>
+      <c r="ON2" t="inlineStr"/>
+      <c r="OO2" t="inlineStr"/>
+      <c r="OP2" t="inlineStr"/>
+      <c r="OQ2" t="inlineStr"/>
+      <c r="OR2" t="inlineStr"/>
+      <c r="OS2" t="inlineStr"/>
+      <c r="OT2" t="inlineStr"/>
+      <c r="OU2" t="inlineStr"/>
+      <c r="OV2" t="inlineStr"/>
+      <c r="OW2" t="inlineStr"/>
+      <c r="OX2" t="inlineStr"/>
+      <c r="OY2" t="inlineStr"/>
+      <c r="OZ2" t="inlineStr"/>
+      <c r="PA2" t="inlineStr"/>
+      <c r="PB2" t="inlineStr"/>
+      <c r="PC2" t="inlineStr"/>
+      <c r="PD2" t="inlineStr"/>
+      <c r="PE2" t="inlineStr"/>
+      <c r="PF2" t="inlineStr"/>
+      <c r="PG2" t="inlineStr"/>
+      <c r="PH2" t="inlineStr"/>
+      <c r="PI2" t="inlineStr"/>
+      <c r="PJ2" t="inlineStr"/>
+      <c r="PK2" t="inlineStr"/>
+      <c r="PL2" t="inlineStr"/>
+      <c r="PM2" t="inlineStr"/>
+      <c r="PN2" t="inlineStr"/>
+      <c r="PO2" t="inlineStr"/>
+      <c r="PP2" t="inlineStr"/>
+      <c r="PQ2" t="inlineStr"/>
+      <c r="PR2" t="inlineStr"/>
+      <c r="PS2" t="inlineStr"/>
+      <c r="PT2" t="inlineStr"/>
+      <c r="PU2" t="inlineStr"/>
+      <c r="PV2" t="inlineStr"/>
+      <c r="PW2" t="inlineStr"/>
+      <c r="PX2" t="inlineStr"/>
+      <c r="PY2" t="inlineStr"/>
+      <c r="PZ2" t="inlineStr"/>
+      <c r="QA2" t="inlineStr"/>
+      <c r="QB2" t="inlineStr"/>
+      <c r="QC2" t="inlineStr"/>
+      <c r="QD2" t="inlineStr"/>
+      <c r="QE2" t="inlineStr"/>
+      <c r="QF2" t="inlineStr"/>
+      <c r="QG2" t="inlineStr"/>
+      <c r="QH2" t="inlineStr"/>
+      <c r="QI2" t="inlineStr"/>
+      <c r="QJ2" t="inlineStr"/>
+      <c r="QK2" t="inlineStr"/>
+      <c r="QL2" t="inlineStr"/>
+      <c r="QM2" t="inlineStr"/>
+      <c r="QN2" t="inlineStr"/>
+      <c r="QO2" t="inlineStr"/>
+      <c r="QP2" t="inlineStr"/>
+      <c r="QQ2" t="inlineStr"/>
+      <c r="QR2" t="inlineStr"/>
+      <c r="QS2" t="inlineStr"/>
+      <c r="QT2" t="inlineStr"/>
+      <c r="QU2" t="inlineStr"/>
+      <c r="QV2" t="inlineStr"/>
+      <c r="QW2" t="inlineStr"/>
+      <c r="QX2" t="inlineStr"/>
+      <c r="QY2" t="inlineStr"/>
+      <c r="QZ2" t="inlineStr"/>
+      <c r="RA2" t="inlineStr"/>
+      <c r="RB2" t="inlineStr"/>
+      <c r="RC2" t="inlineStr"/>
+      <c r="RD2" t="inlineStr"/>
+      <c r="RE2" t="inlineStr"/>
+      <c r="RF2" t="inlineStr"/>
+      <c r="RG2" t="inlineStr"/>
+      <c r="RH2" t="inlineStr"/>
+      <c r="RI2" t="inlineStr"/>
+      <c r="RJ2" t="inlineStr"/>
+      <c r="RK2" t="inlineStr"/>
+      <c r="RL2" t="inlineStr"/>
+      <c r="RM2" t="inlineStr"/>
+      <c r="RN2" t="inlineStr"/>
+      <c r="RO2" t="inlineStr"/>
+      <c r="RP2" t="inlineStr"/>
+      <c r="RQ2" t="inlineStr"/>
+      <c r="RR2" t="inlineStr"/>
+      <c r="RS2" t="inlineStr"/>
+      <c r="RT2" t="inlineStr"/>
+      <c r="RU2" t="inlineStr"/>
+      <c r="RV2" t="inlineStr"/>
+      <c r="RW2" t="inlineStr"/>
+      <c r="RX2" t="inlineStr"/>
+      <c r="RY2" t="inlineStr"/>
+      <c r="RZ2" t="inlineStr"/>
+      <c r="SA2" t="inlineStr"/>
+      <c r="SB2" t="inlineStr"/>
+      <c r="SC2" t="inlineStr"/>
+      <c r="SD2" t="inlineStr"/>
+      <c r="SE2" t="inlineStr"/>
+      <c r="SF2" t="inlineStr"/>
+      <c r="SG2" t="inlineStr"/>
+      <c r="SH2" t="inlineStr"/>
+      <c r="SI2" t="inlineStr"/>
+      <c r="SJ2" t="inlineStr"/>
+      <c r="SK2" t="inlineStr"/>
+      <c r="SL2" t="inlineStr"/>
+      <c r="SM2" t="inlineStr"/>
+      <c r="SN2" t="inlineStr"/>
+      <c r="SO2" t="inlineStr"/>
+      <c r="SP2" t="inlineStr"/>
+      <c r="SQ2" t="inlineStr"/>
+      <c r="SR2" t="inlineStr"/>
+      <c r="SS2" t="inlineStr"/>
+      <c r="ST2" t="inlineStr"/>
+      <c r="SU2" t="inlineStr"/>
+      <c r="SV2" t="inlineStr"/>
+      <c r="SW2" t="inlineStr"/>
+      <c r="SX2" t="inlineStr"/>
+      <c r="SY2" t="inlineStr"/>
+      <c r="SZ2" t="inlineStr"/>
+      <c r="TA2" t="inlineStr"/>
+      <c r="TB2" t="inlineStr"/>
+      <c r="TC2" t="inlineStr"/>
+      <c r="TD2" t="inlineStr"/>
+      <c r="TE2" t="inlineStr"/>
+      <c r="TF2" t="inlineStr"/>
+      <c r="TG2" t="inlineStr"/>
+      <c r="TH2" t="inlineStr"/>
+      <c r="TI2" t="inlineStr"/>
+      <c r="TJ2" t="inlineStr"/>
+      <c r="TK2" t="inlineStr"/>
+      <c r="TL2" t="inlineStr"/>
+      <c r="TM2" t="inlineStr"/>
+      <c r="TN2" t="inlineStr"/>
+      <c r="TO2" t="inlineStr"/>
+      <c r="TP2" t="inlineStr"/>
+      <c r="TQ2" t="inlineStr"/>
+      <c r="TR2" t="inlineStr"/>
+      <c r="TS2" t="inlineStr"/>
+      <c r="TT2" t="inlineStr"/>
+      <c r="TU2" t="inlineStr"/>
+      <c r="TV2" t="inlineStr"/>
+      <c r="TW2" t="inlineStr"/>
+      <c r="TX2" t="inlineStr"/>
+      <c r="TY2" t="inlineStr"/>
+      <c r="TZ2" t="inlineStr"/>
+      <c r="UA2" t="inlineStr"/>
+      <c r="UB2" t="inlineStr"/>
+      <c r="UC2" t="inlineStr"/>
+      <c r="UD2" t="inlineStr"/>
+      <c r="UE2" t="inlineStr"/>
+      <c r="UF2" t="inlineStr"/>
+      <c r="UG2" t="inlineStr"/>
+      <c r="UH2" t="inlineStr"/>
+      <c r="UI2" t="inlineStr"/>
+      <c r="UJ2" t="inlineStr"/>
+      <c r="UK2" t="inlineStr"/>
+      <c r="UL2" t="inlineStr"/>
+      <c r="UM2" t="inlineStr"/>
+      <c r="UN2" t="inlineStr"/>
+      <c r="UO2" t="inlineStr"/>
+      <c r="UP2" t="inlineStr"/>
+      <c r="UQ2" t="inlineStr"/>
+      <c r="UR2" t="inlineStr"/>
+      <c r="US2" t="inlineStr"/>
+      <c r="UT2" t="inlineStr"/>
+      <c r="UU2" t="inlineStr"/>
+      <c r="UV2" t="inlineStr"/>
+      <c r="UW2" t="inlineStr"/>
+      <c r="UX2" t="inlineStr"/>
+      <c r="UY2" t="inlineStr"/>
+      <c r="UZ2" t="inlineStr"/>
+      <c r="VA2" t="inlineStr"/>
+      <c r="VB2" t="inlineStr"/>
+      <c r="VC2" t="inlineStr"/>
+      <c r="VD2" t="inlineStr"/>
+      <c r="VE2" t="inlineStr"/>
+      <c r="VF2" t="inlineStr"/>
+      <c r="VG2" t="inlineStr"/>
+      <c r="VH2" t="inlineStr"/>
+      <c r="VI2" t="inlineStr"/>
+      <c r="VJ2" t="inlineStr"/>
+      <c r="VK2" t="inlineStr"/>
+      <c r="VL2" t="inlineStr"/>
+      <c r="VM2" t="inlineStr"/>
+      <c r="VN2" t="inlineStr"/>
+      <c r="VO2" t="inlineStr"/>
+      <c r="VP2" t="inlineStr"/>
+      <c r="VQ2" t="inlineStr"/>
+      <c r="VR2" t="inlineStr"/>
+      <c r="VS2" t="inlineStr"/>
+      <c r="VT2" t="inlineStr"/>
+      <c r="VU2" t="inlineStr"/>
+      <c r="VV2" t="inlineStr"/>
+      <c r="VW2" t="inlineStr"/>
+      <c r="VX2" t="inlineStr"/>
+      <c r="VY2" t="inlineStr"/>
+      <c r="VZ2" t="inlineStr"/>
+      <c r="WA2" t="inlineStr"/>
+      <c r="WB2" t="inlineStr"/>
+      <c r="WC2" t="inlineStr"/>
+      <c r="WD2" t="inlineStr"/>
+      <c r="WE2" t="inlineStr"/>
+      <c r="WF2" t="inlineStr"/>
+      <c r="WG2" t="inlineStr"/>
+      <c r="WH2" t="inlineStr"/>
+      <c r="WI2" t="inlineStr"/>
+      <c r="WJ2" t="inlineStr"/>
+      <c r="WK2" t="inlineStr"/>
+      <c r="WL2" t="inlineStr"/>
+      <c r="WM2" t="inlineStr"/>
+      <c r="WN2" t="inlineStr"/>
+      <c r="WO2" t="inlineStr"/>
+      <c r="WP2" t="inlineStr"/>
+      <c r="WQ2" t="inlineStr"/>
+      <c r="WR2" t="inlineStr"/>
+      <c r="WS2" t="inlineStr"/>
+      <c r="WT2" t="inlineStr"/>
+      <c r="WU2" t="inlineStr"/>
+      <c r="WV2" t="inlineStr"/>
+      <c r="WW2" t="inlineStr"/>
+      <c r="WX2" t="inlineStr"/>
+      <c r="WY2" t="inlineStr"/>
+      <c r="WZ2" t="inlineStr"/>
+      <c r="XA2" t="inlineStr"/>
+      <c r="XB2" t="inlineStr"/>
+      <c r="XC2" t="inlineStr"/>
+      <c r="XD2" t="inlineStr"/>
+      <c r="XE2" t="inlineStr"/>
+      <c r="XF2" t="inlineStr"/>
+      <c r="XG2" t="inlineStr"/>
+      <c r="XH2" t="inlineStr"/>
+      <c r="XI2" t="inlineStr"/>
+      <c r="XJ2" t="inlineStr"/>
+      <c r="XK2" t="inlineStr"/>
+      <c r="XL2" t="inlineStr"/>
+      <c r="XM2" t="inlineStr"/>
+      <c r="XN2" t="inlineStr"/>
+      <c r="XO2" t="inlineStr"/>
+      <c r="XP2" t="inlineStr"/>
+      <c r="XQ2" t="inlineStr"/>
+      <c r="XR2" t="inlineStr"/>
+      <c r="XS2" t="inlineStr"/>
+      <c r="XT2" t="inlineStr"/>
+      <c r="XU2" t="inlineStr"/>
+      <c r="XV2" t="inlineStr"/>
+      <c r="XW2" t="inlineStr"/>
+      <c r="XX2" t="inlineStr"/>
+      <c r="XY2" t="inlineStr"/>
+      <c r="XZ2" t="inlineStr"/>
+      <c r="YA2" t="inlineStr"/>
+      <c r="YB2" t="inlineStr"/>
+      <c r="YC2" t="inlineStr"/>
+      <c r="YD2" t="inlineStr"/>
+      <c r="YE2" t="inlineStr"/>
+      <c r="YF2" t="inlineStr"/>
+      <c r="YG2" t="inlineStr"/>
+      <c r="YH2" t="inlineStr"/>
+      <c r="YI2" t="inlineStr"/>
+      <c r="YJ2" t="inlineStr"/>
+      <c r="YK2" t="inlineStr"/>
+      <c r="YL2" t="inlineStr"/>
+      <c r="YM2" t="inlineStr"/>
+      <c r="YN2" t="inlineStr"/>
+      <c r="YO2" t="inlineStr"/>
+      <c r="YP2" t="inlineStr"/>
+      <c r="YQ2" t="inlineStr"/>
+      <c r="YR2" t="inlineStr"/>
+      <c r="YS2" t="inlineStr"/>
+      <c r="YT2" t="inlineStr"/>
+      <c r="YU2" t="inlineStr"/>
+      <c r="YV2" t="inlineStr"/>
+      <c r="YW2" t="inlineStr"/>
+      <c r="YX2" t="inlineStr"/>
+      <c r="YY2" t="inlineStr"/>
+      <c r="YZ2" t="inlineStr"/>
+      <c r="ZA2" t="inlineStr"/>
+      <c r="ZB2" t="inlineStr"/>
+      <c r="ZC2" t="inlineStr"/>
+      <c r="ZD2" t="inlineStr"/>
+      <c r="ZE2" t="inlineStr"/>
+      <c r="ZF2" t="inlineStr"/>
+      <c r="ZG2" t="inlineStr"/>
+      <c r="ZH2" t="inlineStr"/>
+      <c r="ZI2" t="inlineStr"/>
+      <c r="ZJ2" t="inlineStr"/>
+      <c r="ZK2" t="inlineStr"/>
+      <c r="ZL2" t="inlineStr"/>
+      <c r="ZM2" t="inlineStr"/>
+      <c r="ZN2" t="inlineStr"/>
+      <c r="ZO2" t="inlineStr"/>
+      <c r="ZP2" t="inlineStr"/>
+      <c r="ZQ2" t="inlineStr"/>
+      <c r="ZR2" t="inlineStr"/>
+      <c r="ZS2" t="inlineStr"/>
+      <c r="ZT2" t="inlineStr"/>
+      <c r="ZU2" t="inlineStr"/>
+      <c r="ZV2" t="inlineStr"/>
+      <c r="ZW2" t="inlineStr"/>
+      <c r="ZX2" t="inlineStr"/>
+      <c r="ZY2" t="inlineStr"/>
+      <c r="ZZ2" t="inlineStr"/>
+      <c r="AAA2" t="inlineStr"/>
+      <c r="AAB2" t="inlineStr"/>
+      <c r="AAC2" t="inlineStr"/>
+      <c r="AAD2" t="inlineStr"/>
+      <c r="AAE2" t="inlineStr"/>
+      <c r="AAF2" t="inlineStr"/>
+      <c r="AAG2" t="inlineStr"/>
+      <c r="AAH2" t="inlineStr"/>
+      <c r="AAI2" t="inlineStr"/>
+      <c r="AAJ2" t="inlineStr"/>
+      <c r="AAK2" t="inlineStr"/>
+      <c r="AAL2" t="inlineStr"/>
+      <c r="AAM2" t="inlineStr"/>
+      <c r="AAN2" t="inlineStr"/>
+      <c r="AAO2" t="inlineStr"/>
+      <c r="AAP2" t="inlineStr"/>
+      <c r="AAQ2" t="inlineStr"/>
+      <c r="AAR2" t="inlineStr"/>
+      <c r="AAS2" t="inlineStr"/>
+      <c r="AAT2" t="inlineStr"/>
+      <c r="AAU2" t="inlineStr"/>
+      <c r="AAV2" t="inlineStr"/>
+      <c r="AAW2" t="inlineStr"/>
+      <c r="AAX2" t="inlineStr"/>
+      <c r="AAY2" t="inlineStr"/>
+      <c r="AAZ2" t="inlineStr"/>
+      <c r="ABA2" t="inlineStr"/>
+      <c r="ABB2" t="inlineStr"/>
+      <c r="ABC2" t="inlineStr"/>
+      <c r="ABD2" t="inlineStr"/>
+      <c r="ABE2" t="inlineStr"/>
+      <c r="ABF2" t="inlineStr"/>
+      <c r="ABG2" t="inlineStr"/>
+      <c r="ABH2" t="inlineStr"/>
+      <c r="ABI2" t="inlineStr"/>
+      <c r="ABJ2" t="inlineStr"/>
+      <c r="ABK2" t="inlineStr"/>
+      <c r="ABL2" t="inlineStr"/>
+      <c r="ABM2" t="inlineStr"/>
+      <c r="ABN2" t="inlineStr"/>
+      <c r="ABO2" t="inlineStr"/>
+      <c r="ABP2" t="inlineStr"/>
+      <c r="ABQ2" t="inlineStr"/>
+      <c r="ABR2" t="inlineStr"/>
+      <c r="ABS2" t="inlineStr"/>
+      <c r="ABT2" t="inlineStr"/>
+      <c r="ABU2" t="inlineStr"/>
+      <c r="ABV2" t="inlineStr"/>
+      <c r="ABW2" t="inlineStr"/>
+      <c r="ABX2" t="inlineStr"/>
+      <c r="ABY2" t="inlineStr"/>
+      <c r="ABZ2" t="inlineStr"/>
+      <c r="ACA2" t="inlineStr"/>
+      <c r="ACB2" t="inlineStr"/>
+      <c r="ACC2" t="inlineStr"/>
+      <c r="ACD2" t="inlineStr"/>
+      <c r="ACE2" t="inlineStr"/>
+      <c r="ACF2" t="inlineStr"/>
+      <c r="ACG2" t="inlineStr"/>
+      <c r="ACH2" t="inlineStr"/>
+      <c r="ACI2" t="inlineStr"/>
+      <c r="ACJ2" t="inlineStr"/>
+      <c r="ACK2" t="inlineStr"/>
+      <c r="ACL2" t="inlineStr"/>
+      <c r="ACM2" t="inlineStr"/>
+      <c r="ACN2" t="inlineStr"/>
+      <c r="ACO2" t="inlineStr"/>
+      <c r="ACP2" t="inlineStr"/>
+      <c r="ACQ2" t="inlineStr"/>
+      <c r="ACR2" t="inlineStr"/>
+      <c r="ACS2" t="inlineStr"/>
+      <c r="ACT2" t="inlineStr"/>
+      <c r="ACU2" t="inlineStr"/>
+      <c r="ACV2" t="inlineStr"/>
+      <c r="ACW2" t="inlineStr"/>
+      <c r="ACX2" t="inlineStr"/>
+      <c r="ACY2" t="inlineStr"/>
+      <c r="ACZ2" t="inlineStr"/>
+      <c r="ADA2" t="inlineStr"/>
+      <c r="ADB2" t="inlineStr"/>
+      <c r="ADC2" t="inlineStr"/>
+      <c r="ADD2" t="inlineStr"/>
+      <c r="ADE2" t="inlineStr"/>
+      <c r="ADF2" t="inlineStr"/>
+      <c r="ADG2" t="inlineStr"/>
+      <c r="ADH2" t="inlineStr"/>
+      <c r="ADI2" t="inlineStr"/>
+      <c r="ADJ2" t="inlineStr"/>
+      <c r="ADK2" t="inlineStr"/>
+      <c r="ADL2" t="inlineStr"/>
+      <c r="ADM2" t="inlineStr"/>
+      <c r="ADN2" t="inlineStr"/>
+      <c r="ADO2" t="inlineStr"/>
+      <c r="ADP2" t="inlineStr"/>
+      <c r="ADQ2" t="inlineStr"/>
+      <c r="ADR2" t="inlineStr"/>
+      <c r="ADS2" t="inlineStr"/>
+      <c r="ADT2" t="inlineStr"/>
+      <c r="ADU2" t="inlineStr"/>
+      <c r="ADV2" t="inlineStr"/>
+      <c r="ADW2" t="inlineStr"/>
+      <c r="ADX2" t="inlineStr"/>
+      <c r="ADY2" t="inlineStr"/>
+      <c r="ADZ2" t="inlineStr"/>
+      <c r="AEA2" t="inlineStr"/>
+      <c r="AEB2" t="inlineStr"/>
+      <c r="AEC2" t="inlineStr"/>
+      <c r="AED2" t="inlineStr"/>
+      <c r="AEE2" t="inlineStr"/>
+      <c r="AEF2" t="inlineStr"/>
+      <c r="AEG2" t="inlineStr"/>
+      <c r="AEH2" t="inlineStr"/>
+      <c r="AEI2" t="inlineStr"/>
+      <c r="AEJ2" t="inlineStr"/>
+      <c r="AEK2" t="inlineStr"/>
+      <c r="AEL2" t="inlineStr"/>
+      <c r="AEM2" t="inlineStr"/>
+      <c r="AEN2" t="inlineStr"/>
+      <c r="AEO2" t="inlineStr"/>
+      <c r="AEP2" t="inlineStr"/>
+      <c r="AEQ2" t="inlineStr"/>
+      <c r="AER2" t="inlineStr"/>
+      <c r="AES2" t="inlineStr"/>
+      <c r="AET2" t="inlineStr"/>
+      <c r="AEU2" t="inlineStr"/>
+      <c r="AEV2" t="inlineStr"/>
+      <c r="AEW2" t="inlineStr"/>
+      <c r="AEX2" t="inlineStr"/>
+      <c r="AEY2" t="inlineStr"/>
+      <c r="AEZ2" t="inlineStr"/>
+      <c r="AFA2" t="inlineStr"/>
+      <c r="AFB2" t="inlineStr"/>
+      <c r="AFC2" t="inlineStr"/>
+      <c r="AFD2" t="inlineStr"/>
+      <c r="AFE2" t="inlineStr"/>
+      <c r="AFF2" t="inlineStr"/>
+      <c r="AFG2" t="inlineStr"/>
+      <c r="AFH2" t="inlineStr"/>
+      <c r="AFI2" t="inlineStr"/>
+      <c r="AFJ2" t="inlineStr"/>
+      <c r="AFK2" t="inlineStr"/>
+      <c r="AFL2" t="inlineStr"/>
+      <c r="AFM2" t="inlineStr"/>
+      <c r="AFN2" t="inlineStr"/>
+      <c r="AFO2" t="inlineStr"/>
+      <c r="AFP2" t="inlineStr"/>
+      <c r="AFQ2" t="inlineStr"/>
+      <c r="AFR2" t="inlineStr"/>
+      <c r="AFS2" t="inlineStr"/>
+      <c r="AFT2" t="inlineStr"/>
+      <c r="AFU2" t="inlineStr"/>
+      <c r="AFV2" t="inlineStr"/>
+      <c r="AFW2" t="inlineStr"/>
+      <c r="AFX2" t="inlineStr"/>
+      <c r="AFY2" t="inlineStr"/>
+      <c r="AFZ2" t="inlineStr"/>
+      <c r="AGA2" t="inlineStr"/>
+      <c r="AGB2" t="inlineStr"/>
+      <c r="AGC2" t="inlineStr"/>
+      <c r="AGD2" t="inlineStr"/>
+      <c r="AGE2" t="inlineStr"/>
+      <c r="AGF2" t="inlineStr"/>
+      <c r="AGG2" t="inlineStr"/>
+      <c r="AGH2" t="inlineStr"/>
+      <c r="AGI2" t="inlineStr"/>
+      <c r="AGJ2" t="inlineStr"/>
+      <c r="AGK2" t="inlineStr"/>
+      <c r="AGL2" t="inlineStr"/>
+      <c r="AGM2" t="inlineStr"/>
+      <c r="AGN2" t="inlineStr"/>
+      <c r="AGO2" t="inlineStr"/>
+      <c r="AGP2" t="inlineStr"/>
+      <c r="AGQ2" t="inlineStr"/>
+      <c r="AGR2" t="inlineStr"/>
+      <c r="AGS2" t="inlineStr"/>
+      <c r="AGT2" t="inlineStr"/>
+      <c r="AGU2" t="inlineStr"/>
+      <c r="AGV2" t="inlineStr"/>
+      <c r="AGW2" t="inlineStr"/>
+      <c r="AGX2" t="inlineStr"/>
+      <c r="AGY2" t="inlineStr"/>
+      <c r="AGZ2" t="inlineStr"/>
+      <c r="AHA2" t="inlineStr"/>
+      <c r="AHB2" t="inlineStr"/>
+      <c r="AHC2" t="inlineStr"/>
+      <c r="AHD2" t="inlineStr"/>
+      <c r="AHE2" t="inlineStr"/>
+      <c r="AHF2" t="inlineStr"/>
+      <c r="AHG2" t="inlineStr"/>
+      <c r="AHH2" t="inlineStr"/>
+      <c r="AHI2" t="inlineStr"/>
+      <c r="AHJ2" t="inlineStr"/>
+      <c r="AHK2" t="inlineStr"/>
+      <c r="AHL2" t="inlineStr"/>
+      <c r="AHM2" t="inlineStr"/>
+      <c r="AHN2" t="inlineStr"/>
+      <c r="AHO2" t="inlineStr"/>
+      <c r="AHP2" t="inlineStr"/>
+      <c r="AHQ2" t="inlineStr"/>
+      <c r="AHR2" t="inlineStr"/>
+      <c r="AHS2" t="inlineStr"/>
+      <c r="AHT2" t="inlineStr"/>
+      <c r="AHU2" t="inlineStr"/>
+      <c r="AHV2" t="inlineStr"/>
+      <c r="AHW2" t="inlineStr"/>
+      <c r="AHX2" t="inlineStr"/>
+      <c r="AHY2" t="inlineStr"/>
+      <c r="AHZ2" t="inlineStr"/>
+      <c r="AIA2" t="inlineStr"/>
+      <c r="AIB2" t="inlineStr"/>
+      <c r="AIC2" t="inlineStr"/>
+      <c r="AID2" t="inlineStr"/>
+      <c r="AIE2" t="inlineStr"/>
+      <c r="AIF2" t="inlineStr"/>
+      <c r="AIG2" t="inlineStr"/>
+      <c r="AIH2" t="inlineStr"/>
+      <c r="AII2" t="inlineStr"/>
+      <c r="AIJ2" t="inlineStr"/>
+      <c r="AIK2" t="inlineStr"/>
+      <c r="AIL2" t="inlineStr"/>
+      <c r="AIM2" t="inlineStr"/>
+      <c r="AIN2" t="inlineStr"/>
+      <c r="AIO2" t="inlineStr"/>
+      <c r="AIP2" t="inlineStr"/>
+      <c r="AIQ2" t="inlineStr"/>
+      <c r="AIR2" t="inlineStr"/>
+      <c r="AIS2" t="inlineStr"/>
+      <c r="AIT2" t="inlineStr"/>
+      <c r="AIU2" t="inlineStr"/>
+      <c r="AIV2" t="inlineStr"/>
+      <c r="AIW2" t="inlineStr"/>
+      <c r="AIX2" t="inlineStr"/>
+      <c r="AIY2" t="inlineStr"/>
+      <c r="AIZ2" t="inlineStr"/>
+      <c r="AJA2" t="inlineStr"/>
+      <c r="AJB2" t="inlineStr"/>
+      <c r="AJC2" t="inlineStr"/>
+      <c r="AJD2" t="inlineStr"/>
+      <c r="AJE2" t="inlineStr"/>
+      <c r="AJF2" t="inlineStr"/>
+      <c r="AJG2" t="inlineStr"/>
+      <c r="AJH2" t="inlineStr"/>
+      <c r="AJI2" t="inlineStr"/>
+      <c r="AJJ2" t="inlineStr"/>
+      <c r="AJK2" t="inlineStr"/>
+      <c r="AJL2" t="inlineStr"/>
+      <c r="AJM2" t="inlineStr"/>
+      <c r="AJN2" t="inlineStr"/>
+      <c r="AJO2" t="inlineStr"/>
+      <c r="AJP2" t="inlineStr"/>
+      <c r="AJQ2" t="inlineStr"/>
+      <c r="AJR2" t="inlineStr"/>
+      <c r="AJS2" t="inlineStr"/>
+      <c r="AJT2" t="inlineStr"/>
+      <c r="AJU2" t="inlineStr"/>
+      <c r="AJV2" t="inlineStr"/>
+      <c r="AJW2" t="inlineStr"/>
+      <c r="AJX2" t="inlineStr"/>
+      <c r="AJY2" t="inlineStr"/>
+      <c r="AJZ2" t="inlineStr"/>
+      <c r="AKA2" t="inlineStr"/>
+      <c r="AKB2" t="inlineStr"/>
+      <c r="AKC2" t="inlineStr"/>
+      <c r="AKD2" t="inlineStr"/>
+      <c r="AKE2" t="inlineStr"/>
+      <c r="AKF2" t="inlineStr"/>
+      <c r="AKG2" t="inlineStr"/>
+      <c r="AKH2" t="inlineStr"/>
+      <c r="AKI2" t="inlineStr"/>
+      <c r="AKJ2" t="inlineStr"/>
+      <c r="AKK2" t="inlineStr"/>
+      <c r="AKL2" t="inlineStr"/>
+      <c r="AKM2" t="inlineStr"/>
+      <c r="AKN2" t="inlineStr"/>
+      <c r="AKO2" t="inlineStr"/>
+      <c r="AKP2" t="inlineStr"/>
+      <c r="AKQ2" t="inlineStr"/>
+      <c r="AKR2" t="inlineStr"/>
+      <c r="AKS2" t="inlineStr"/>
+      <c r="AKT2" t="inlineStr"/>
+      <c r="AKU2" t="inlineStr"/>
+      <c r="AKV2" t="inlineStr"/>
+      <c r="AKW2" t="inlineStr"/>
+      <c r="AKX2" t="inlineStr"/>
+      <c r="AKY2" t="inlineStr"/>
+      <c r="AKZ2" t="inlineStr"/>
+      <c r="ALA2" t="inlineStr"/>
+      <c r="ALB2" t="inlineStr"/>
+      <c r="ALC2" t="inlineStr"/>
+      <c r="ALD2" t="inlineStr"/>
+      <c r="ALE2" t="inlineStr"/>
+      <c r="ALF2" t="inlineStr"/>
+      <c r="ALG2" t="inlineStr"/>
+      <c r="ALH2" t="inlineStr"/>
+      <c r="ALI2" t="inlineStr"/>
+      <c r="ALJ2" t="inlineStr"/>
+      <c r="ALK2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>